<commit_message>
working on limiting on incrementing
</commit_message>
<xml_diff>
--- a/docs/Costs and pricing-LOCAL.xlsx
+++ b/docs/Costs and pricing-LOCAL.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648"/>
   </bookViews>
   <sheets>
     <sheet name="BOYOUTI" sheetId="1" r:id="rId1"/>
@@ -1001,10 +1001,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AB40"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="B24" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane xSplit="1" topLeftCell="C1" activePane="topRight" state="frozen"/>
       <selection activeCell="B1" sqref="B1"/>
-      <selection pane="topRight" activeCell="D3" sqref="D3"/>
+      <selection pane="topRight" activeCell="G25" sqref="G25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3310,7 +3310,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AB39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView topLeftCell="B1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane xSplit="1" topLeftCell="C1" activePane="topRight" state="frozen"/>
       <selection activeCell="B1" sqref="B1"/>
       <selection pane="topRight" activeCell="G7" sqref="G7"/>
@@ -3493,7 +3493,7 @@
         <v>10500</v>
       </c>
       <c r="K5" s="6">
-        <f>(J5/$J$31)*$M$2</f>
+        <f t="shared" ref="K5:K30" si="1">(J5/$J$31)*$M$2</f>
         <v>149.3099121706399</v>
       </c>
       <c r="L5" s="6">
@@ -3501,7 +3501,7 @@
         <v>10649.30991217064</v>
       </c>
       <c r="M5" s="6">
-        <f t="shared" ref="M5:M30" si="1">+L5/C5</f>
+        <f t="shared" ref="M5:M30" si="2">+L5/C5</f>
         <v>354.97699707235466</v>
       </c>
       <c r="N5" s="6">
@@ -3518,7 +3518,7 @@
         <v>18</v>
       </c>
       <c r="R5" s="6">
-        <f>((L5/$L$31)*$P$2)/C5</f>
+        <f t="shared" ref="R5:R30" si="3">((L5/$L$31)*$P$2)/C5</f>
         <v>202.00752823086574</v>
       </c>
       <c r="S5" s="2"/>
@@ -3537,11 +3537,11 @@
         <v>1400</v>
       </c>
       <c r="AA5" s="10">
-        <f t="shared" ref="AA5:AA30" si="2">(Z5-M5-R5-P5)*C5</f>
+        <f t="shared" ref="AA5:AA30" si="4">(Z5-M5-R5-P5)*C5</f>
         <v>10290.464240903388</v>
       </c>
       <c r="AB5" s="11">
-        <f t="shared" ref="AB5:AB30" si="3">IFERROR(AA5/(M5+P5+R5*C5),"")</f>
+        <f t="shared" ref="AB5:AB30" si="5">IFERROR(AA5/(M5+P5+R5*C5),"")</f>
         <v>1.4880928980752075</v>
       </c>
     </row>
@@ -3572,19 +3572,19 @@
         <v>4050</v>
       </c>
       <c r="K6" s="6">
-        <f>(J6/$J$31)*$M$2</f>
+        <f t="shared" si="1"/>
         <v>57.590966122961106</v>
       </c>
       <c r="L6" s="6">
-        <f t="shared" ref="L6:L30" si="4">(J6+K6)</f>
+        <f t="shared" ref="L6:L30" si="6">(J6+K6)</f>
         <v>4107.5909661229607</v>
       </c>
       <c r="M6" s="6">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1369.1969887076536</v>
       </c>
       <c r="N6" s="6">
-        <f t="shared" ref="N6:N30" si="5">+M6*0.5</f>
+        <f t="shared" ref="N6:N30" si="7">+M6*0.5</f>
         <v>684.59849435382682</v>
       </c>
       <c r="O6" s="8" t="s">
@@ -3597,13 +3597,13 @@
         <v>18</v>
       </c>
       <c r="R6" s="6">
-        <f>((L6/$L$31)*$P$2)/C6</f>
+        <f t="shared" si="3"/>
         <v>779.17189460476777</v>
       </c>
       <c r="S6" s="2"/>
       <c r="T6" s="7"/>
       <c r="U6" s="17">
-        <f t="shared" ref="U6:U30" si="6">M6+P6+R6+S6+N6</f>
+        <f t="shared" ref="U6:U30" si="8">M6+P6+R6+S6+N6</f>
         <v>3332.9673776662485</v>
       </c>
       <c r="V6" s="6"/>
@@ -3616,11 +3616,11 @@
         <v>1300</v>
       </c>
       <c r="AA6" s="10">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>-4045.1066499372646</v>
       </c>
       <c r="AB6" s="11">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>-0.96158377451345922</v>
       </c>
     </row>
@@ -3651,19 +3651,19 @@
         <v>87000</v>
       </c>
       <c r="K7" s="6">
-        <f>(J7/$J$31)*$M$2</f>
+        <f t="shared" si="1"/>
         <v>1237.1392722710164</v>
       </c>
       <c r="L7" s="6">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>88237.139272271015</v>
       </c>
       <c r="M7" s="6">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>5882.4759514847347</v>
       </c>
       <c r="N7" s="6">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>2941.2379757423673</v>
       </c>
       <c r="O7" s="8" t="s">
@@ -3676,13 +3676,13 @@
         <v>18</v>
       </c>
       <c r="R7" s="6">
-        <f>((L7/$L$31)*$P$2)/C7</f>
+        <f t="shared" si="3"/>
         <v>3347.5533249686323</v>
       </c>
       <c r="S7" s="2"/>
       <c r="T7" s="7"/>
       <c r="U7" s="17">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>12671.267252195734</v>
       </c>
       <c r="V7" s="6"/>
@@ -3693,11 +3693,11 @@
         <v>900</v>
       </c>
       <c r="AA7" s="10">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>-132450.43914680049</v>
       </c>
       <c r="AB7" s="11">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>-2.3402884263655546</v>
       </c>
     </row>
@@ -3728,19 +3728,19 @@
         <v>18000</v>
       </c>
       <c r="K8" s="6">
-        <f>(J8/$J$31)*$M$2</f>
+        <f t="shared" si="1"/>
         <v>255.95984943538267</v>
       </c>
       <c r="L8" s="6">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>18255.959849435381</v>
       </c>
       <c r="M8" s="6">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1825.595984943538</v>
       </c>
       <c r="N8" s="6">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>912.79799247176902</v>
       </c>
       <c r="O8" s="8" t="s">
@@ -3753,13 +3753,13 @@
         <v>18</v>
       </c>
       <c r="R8" s="6">
-        <f>((L8/$L$31)*$P$2)/C8</f>
+        <f t="shared" si="3"/>
         <v>1038.8958594730238</v>
       </c>
       <c r="S8" s="2"/>
       <c r="T8" s="7"/>
       <c r="U8" s="17">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>4277.2898368883307</v>
       </c>
       <c r="V8" s="6"/>
@@ -3772,11 +3772,11 @@
         <v>8500</v>
       </c>
       <c r="AA8" s="10">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>51355.081555834375</v>
       </c>
       <c r="AB8" s="11">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>4.0390783046331471</v>
       </c>
     </row>
@@ -3799,19 +3799,19 @@
         <v>0</v>
       </c>
       <c r="K9" s="6">
-        <f>(J9/$J$31)*$M$2</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="L9" s="6">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="M9" s="6" t="e">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
       <c r="N9" s="6" t="e">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>#DIV/0!</v>
       </c>
       <c r="O9" s="8" t="s">
@@ -3824,13 +3824,13 @@
         <v>18</v>
       </c>
       <c r="R9" s="6" t="e">
-        <f>((L9/$L$31)*$P$2)/C9</f>
+        <f t="shared" si="3"/>
         <v>#DIV/0!</v>
       </c>
       <c r="S9" s="2"/>
       <c r="T9" s="7"/>
       <c r="U9" s="17" t="e">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>#DIV/0!</v>
       </c>
       <c r="V9" s="6"/>
@@ -3841,11 +3841,11 @@
         <v>1400</v>
       </c>
       <c r="AA9" s="10" t="e">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>#DIV/0!</v>
       </c>
       <c r="AB9" s="11" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v/>
       </c>
     </row>
@@ -3868,19 +3868,19 @@
         <v>0</v>
       </c>
       <c r="K10" s="6">
-        <f>(J10/$J$31)*$M$2</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="L10" s="6">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="M10" s="6" t="e">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
       <c r="N10" s="6" t="e">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>#DIV/0!</v>
       </c>
       <c r="O10" s="8" t="s">
@@ -3893,13 +3893,13 @@
         <v>18</v>
       </c>
       <c r="R10" s="6" t="e">
-        <f>((L10/$L$31)*$P$2)/C10</f>
+        <f t="shared" si="3"/>
         <v>#DIV/0!</v>
       </c>
       <c r="S10" s="2"/>
       <c r="T10" s="7"/>
       <c r="U10" s="17" t="e">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>#DIV/0!</v>
       </c>
       <c r="V10" s="6"/>
@@ -3910,11 +3910,11 @@
         <v>1100</v>
       </c>
       <c r="AA10" s="10" t="e">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>#DIV/0!</v>
       </c>
       <c r="AB10" s="11" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v/>
       </c>
     </row>
@@ -3937,19 +3937,19 @@
         <v>0</v>
       </c>
       <c r="K11" s="6">
-        <f>(J11/$J$31)*$M$2</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="L11" s="6">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="M11" s="6" t="e">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
       <c r="N11" s="6" t="e">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>#DIV/0!</v>
       </c>
       <c r="O11" s="8" t="s">
@@ -3962,13 +3962,13 @@
         <v>18</v>
       </c>
       <c r="R11" s="6" t="e">
-        <f>((L11/$L$31)*$P$2)/C11</f>
+        <f t="shared" si="3"/>
         <v>#DIV/0!</v>
       </c>
       <c r="S11" s="2"/>
       <c r="T11" s="7"/>
       <c r="U11" s="17" t="e">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>#DIV/0!</v>
       </c>
       <c r="V11" s="6"/>
@@ -3979,11 +3979,11 @@
         <v>1200</v>
       </c>
       <c r="AA11" s="10" t="e">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>#DIV/0!</v>
       </c>
       <c r="AB11" s="11" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v/>
       </c>
     </row>
@@ -4004,19 +4004,19 @@
         <v>0</v>
       </c>
       <c r="K12" s="6">
-        <f>(J12/$J$31)*$M$2</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="L12" s="6">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="M12" s="6" t="e">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
       <c r="N12" s="6" t="e">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>#DIV/0!</v>
       </c>
       <c r="O12" s="8" t="s">
@@ -4029,13 +4029,13 @@
         <v>18</v>
       </c>
       <c r="R12" s="6" t="e">
-        <f>((L12/$L$31)*$P$2)/C12</f>
+        <f t="shared" si="3"/>
         <v>#DIV/0!</v>
       </c>
       <c r="S12" s="2"/>
       <c r="T12" s="7"/>
       <c r="U12" s="17" t="e">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>#DIV/0!</v>
       </c>
       <c r="V12" s="6"/>
@@ -4046,11 +4046,11 @@
         <v>1350</v>
       </c>
       <c r="AA12" s="10" t="e">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>#DIV/0!</v>
       </c>
       <c r="AB12" s="11" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v/>
       </c>
     </row>
@@ -4073,19 +4073,19 @@
         <v>0</v>
       </c>
       <c r="K13" s="6">
-        <f>(J13/$J$31)*$M$2</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="L13" s="6">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="M13" s="6" t="e">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
       <c r="N13" s="6" t="e">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>#DIV/0!</v>
       </c>
       <c r="O13" s="8" t="s">
@@ -4098,13 +4098,13 @@
         <v>18</v>
       </c>
       <c r="R13" s="6" t="e">
-        <f>((L13/$L$31)*$P$2)/C13</f>
+        <f t="shared" si="3"/>
         <v>#DIV/0!</v>
       </c>
       <c r="S13" s="2"/>
       <c r="T13" s="7"/>
       <c r="U13" s="17" t="e">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>#DIV/0!</v>
       </c>
       <c r="V13" s="6"/>
@@ -4115,11 +4115,11 @@
         <v>1700</v>
       </c>
       <c r="AA13" s="10" t="e">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>#DIV/0!</v>
       </c>
       <c r="AB13" s="11" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v/>
       </c>
     </row>
@@ -4142,19 +4142,19 @@
         <v>0</v>
       </c>
       <c r="K14" s="6">
-        <f>(J14/$J$31)*$M$2</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="L14" s="6">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="M14" s="6" t="e">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
       <c r="N14" s="6" t="e">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>#DIV/0!</v>
       </c>
       <c r="O14" s="8" t="s">
@@ -4167,13 +4167,13 @@
         <v>18</v>
       </c>
       <c r="R14" s="6" t="e">
-        <f>((L14/$L$31)*$P$2)/C14</f>
+        <f t="shared" si="3"/>
         <v>#DIV/0!</v>
       </c>
       <c r="S14" s="2"/>
       <c r="T14" s="7"/>
       <c r="U14" s="17" t="e">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>#DIV/0!</v>
       </c>
       <c r="V14" s="6"/>
@@ -4184,11 +4184,11 @@
         <v>1900</v>
       </c>
       <c r="AA14" s="10" t="e">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>#DIV/0!</v>
       </c>
       <c r="AB14" s="11" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v/>
       </c>
     </row>
@@ -4211,19 +4211,19 @@
         <v>0</v>
       </c>
       <c r="K15" s="6">
-        <f>(J15/$J$31)*$M$2</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="L15" s="6">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="M15" s="6" t="e">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
       <c r="N15" s="6" t="e">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>#DIV/0!</v>
       </c>
       <c r="O15" s="8" t="s">
@@ -4236,13 +4236,13 @@
         <v>18</v>
       </c>
       <c r="R15" s="6" t="e">
-        <f>((L15/$L$31)*$P$2)/C15</f>
+        <f t="shared" si="3"/>
         <v>#DIV/0!</v>
       </c>
       <c r="S15" s="2"/>
       <c r="T15" s="7"/>
       <c r="U15" s="17" t="e">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>#DIV/0!</v>
       </c>
       <c r="V15" s="6"/>
@@ -4253,11 +4253,11 @@
         <v>1800</v>
       </c>
       <c r="AA15" s="10" t="e">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>#DIV/0!</v>
       </c>
       <c r="AB15" s="11" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v/>
       </c>
     </row>
@@ -4280,19 +4280,19 @@
         <v>0</v>
       </c>
       <c r="K16" s="6">
-        <f>(J16/$J$31)*$M$2</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="L16" s="6">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="M16" s="6" t="e">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
       <c r="N16" s="6" t="e">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>#DIV/0!</v>
       </c>
       <c r="O16" s="8" t="s">
@@ -4305,13 +4305,13 @@
         <v>18</v>
       </c>
       <c r="R16" s="6" t="e">
-        <f>((L16/$L$31)*$P$2)/C16</f>
+        <f t="shared" si="3"/>
         <v>#DIV/0!</v>
       </c>
       <c r="S16" s="2"/>
       <c r="T16" s="7"/>
       <c r="U16" s="17" t="e">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>#DIV/0!</v>
       </c>
       <c r="V16" s="6"/>
@@ -4322,11 +4322,11 @@
         <v>2600</v>
       </c>
       <c r="AA16" s="10" t="e">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>#DIV/0!</v>
       </c>
       <c r="AB16" s="11" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v/>
       </c>
     </row>
@@ -4349,19 +4349,19 @@
         <v>0</v>
       </c>
       <c r="K17" s="6">
-        <f>(J17/$J$31)*$M$2</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="L17" s="6">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="M17" s="6" t="e">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
       <c r="N17" s="6" t="e">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>#DIV/0!</v>
       </c>
       <c r="O17" s="8" t="s">
@@ -4374,13 +4374,13 @@
         <v>18</v>
       </c>
       <c r="R17" s="6" t="e">
-        <f>((L17/$L$31)*$P$2)/C17</f>
+        <f t="shared" si="3"/>
         <v>#DIV/0!</v>
       </c>
       <c r="S17" s="2"/>
       <c r="T17" s="7"/>
       <c r="U17" s="17" t="e">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>#DIV/0!</v>
       </c>
       <c r="V17" s="6"/>
@@ -4391,11 +4391,11 @@
         <v>1100</v>
       </c>
       <c r="AA17" s="10" t="e">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>#DIV/0!</v>
       </c>
       <c r="AB17" s="11" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v/>
       </c>
     </row>
@@ -4418,19 +4418,19 @@
         <v>0</v>
       </c>
       <c r="K18" s="6">
-        <f>(J18/$J$31)*$M$2</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="L18" s="6">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="M18" s="6" t="e">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
       <c r="N18" s="6" t="e">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>#DIV/0!</v>
       </c>
       <c r="O18" s="8" t="s">
@@ -4443,13 +4443,13 @@
         <v>18</v>
       </c>
       <c r="R18" s="6" t="e">
-        <f>((L18/$L$31)*$P$2)/C18</f>
+        <f t="shared" si="3"/>
         <v>#DIV/0!</v>
       </c>
       <c r="S18" s="2"/>
       <c r="T18" s="7"/>
       <c r="U18" s="17" t="e">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>#DIV/0!</v>
       </c>
       <c r="V18" s="6"/>
@@ -4460,11 +4460,11 @@
         <v>2300</v>
       </c>
       <c r="AA18" s="10" t="e">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>#DIV/0!</v>
       </c>
       <c r="AB18" s="11" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v/>
       </c>
     </row>
@@ -4487,19 +4487,19 @@
         <v>0</v>
       </c>
       <c r="K19" s="6">
-        <f>(J19/$J$31)*$M$2</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="L19" s="6">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="M19" s="6" t="e">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
       <c r="N19" s="6" t="e">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>#DIV/0!</v>
       </c>
       <c r="O19" s="8" t="s">
@@ -4512,13 +4512,13 @@
         <v>18</v>
       </c>
       <c r="R19" s="6" t="e">
-        <f>((L19/$L$31)*$P$2)/C19</f>
+        <f t="shared" si="3"/>
         <v>#DIV/0!</v>
       </c>
       <c r="S19" s="2"/>
       <c r="T19" s="7"/>
       <c r="U19" s="17" t="e">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>#DIV/0!</v>
       </c>
       <c r="V19" s="6"/>
@@ -4529,11 +4529,11 @@
         <v>1100</v>
       </c>
       <c r="AA19" s="10" t="e">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>#DIV/0!</v>
       </c>
       <c r="AB19" s="11" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v/>
       </c>
     </row>
@@ -4556,19 +4556,19 @@
         <v>0</v>
       </c>
       <c r="K20" s="6">
-        <f>(J20/$J$31)*$M$2</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="L20" s="6">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="M20" s="6" t="e">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
       <c r="N20" s="6" t="e">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>#DIV/0!</v>
       </c>
       <c r="O20" s="8" t="s">
@@ -4581,13 +4581,13 @@
         <v>18</v>
       </c>
       <c r="R20" s="6" t="e">
-        <f>((L20/$L$31)*$P$2)/C20</f>
+        <f t="shared" si="3"/>
         <v>#DIV/0!</v>
       </c>
       <c r="S20" s="2"/>
       <c r="T20" s="7"/>
       <c r="U20" s="17" t="e">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>#DIV/0!</v>
       </c>
       <c r="V20" s="6"/>
@@ -4598,11 +4598,11 @@
         <v>700</v>
       </c>
       <c r="AA20" s="10" t="e">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>#DIV/0!</v>
       </c>
       <c r="AB20" s="11" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v/>
       </c>
     </row>
@@ -4625,19 +4625,19 @@
         <v>0</v>
       </c>
       <c r="K21" s="6">
-        <f>(J21/$J$31)*$M$2</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="L21" s="6">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="M21" s="6" t="e">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
       <c r="N21" s="6" t="e">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>#DIV/0!</v>
       </c>
       <c r="O21" s="8" t="s">
@@ -4650,13 +4650,13 @@
         <v>18</v>
       </c>
       <c r="R21" s="6" t="e">
-        <f>((L21/$L$31)*$P$2)/C21</f>
+        <f t="shared" si="3"/>
         <v>#DIV/0!</v>
       </c>
       <c r="S21" s="2"/>
       <c r="T21" s="7"/>
       <c r="U21" s="17" t="e">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>#DIV/0!</v>
       </c>
       <c r="V21" s="6"/>
@@ -4667,11 +4667,11 @@
         <v>800</v>
       </c>
       <c r="AA21" s="10" t="e">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>#DIV/0!</v>
       </c>
       <c r="AB21" s="11" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v/>
       </c>
     </row>
@@ -4694,19 +4694,19 @@
         <v>0</v>
       </c>
       <c r="K22" s="6">
-        <f>(J22/$J$31)*$M$2</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="L22" s="6">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="M22" s="6" t="e">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
       <c r="N22" s="6" t="e">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>#DIV/0!</v>
       </c>
       <c r="O22" s="8" t="s">
@@ -4719,13 +4719,13 @@
         <v>18</v>
       </c>
       <c r="R22" s="6" t="e">
-        <f>((L22/$L$31)*$P$2)/C22</f>
+        <f t="shared" si="3"/>
         <v>#DIV/0!</v>
       </c>
       <c r="S22" s="2"/>
       <c r="T22" s="7"/>
       <c r="U22" s="17" t="e">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>#DIV/0!</v>
       </c>
       <c r="V22" s="6"/>
@@ -4736,11 +4736,11 @@
         <v>800</v>
       </c>
       <c r="AA22" s="10" t="e">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>#DIV/0!</v>
       </c>
       <c r="AB22" s="11" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v/>
       </c>
     </row>
@@ -4763,19 +4763,19 @@
         <v>0</v>
       </c>
       <c r="K23" s="6">
-        <f>(J23/$J$31)*$M$2</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="L23" s="6">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="M23" s="6" t="e">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
       <c r="N23" s="6" t="e">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>#DIV/0!</v>
       </c>
       <c r="O23" s="8" t="s">
@@ -4788,13 +4788,13 @@
         <v>18</v>
       </c>
       <c r="R23" s="6" t="e">
-        <f>((L23/$L$31)*$P$2)/C23</f>
+        <f t="shared" si="3"/>
         <v>#DIV/0!</v>
       </c>
       <c r="S23" s="2"/>
       <c r="T23" s="7"/>
       <c r="U23" s="17" t="e">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>#DIV/0!</v>
       </c>
       <c r="V23" s="6"/>
@@ -4805,11 +4805,11 @@
         <v>1100</v>
       </c>
       <c r="AA23" s="10" t="e">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>#DIV/0!</v>
       </c>
       <c r="AB23" s="11" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v/>
       </c>
     </row>
@@ -4832,19 +4832,19 @@
         <v>0</v>
       </c>
       <c r="K24" s="6">
-        <f>(J24/$J$31)*$M$2</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="L24" s="6">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="M24" s="6" t="e">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
       <c r="N24" s="6" t="e">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>#DIV/0!</v>
       </c>
       <c r="O24" s="8" t="s">
@@ -4857,13 +4857,13 @@
         <v>18</v>
       </c>
       <c r="R24" s="6" t="e">
-        <f>((L24/$L$31)*$P$2)/C24</f>
+        <f t="shared" si="3"/>
         <v>#DIV/0!</v>
       </c>
       <c r="S24" s="2"/>
       <c r="T24" s="7"/>
       <c r="U24" s="17" t="e">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>#DIV/0!</v>
       </c>
       <c r="V24" s="6"/>
@@ -4874,11 +4874,11 @@
         <v>5400</v>
       </c>
       <c r="AA24" s="10" t="e">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>#DIV/0!</v>
       </c>
       <c r="AB24" s="11" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v/>
       </c>
     </row>
@@ -4901,19 +4901,19 @@
         <v>0</v>
       </c>
       <c r="K25" s="6">
-        <f>(J25/$J$31)*$M$2</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="L25" s="6">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="M25" s="6" t="e">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
       <c r="N25" s="6" t="e">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>#DIV/0!</v>
       </c>
       <c r="O25" s="8" t="s">
@@ -4926,13 +4926,13 @@
         <v>18</v>
       </c>
       <c r="R25" s="6" t="e">
-        <f>((L25/$L$31)*$P$2)/C25</f>
+        <f t="shared" si="3"/>
         <v>#DIV/0!</v>
       </c>
       <c r="S25" s="2"/>
       <c r="T25" s="7"/>
       <c r="U25" s="17" t="e">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>#DIV/0!</v>
       </c>
       <c r="V25" s="6"/>
@@ -4943,11 +4943,11 @@
         <v>6500</v>
       </c>
       <c r="AA25" s="10" t="e">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>#DIV/0!</v>
       </c>
       <c r="AB25" s="11" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v/>
       </c>
     </row>
@@ -4970,19 +4970,19 @@
         <v>0</v>
       </c>
       <c r="K26" s="6">
-        <f>(J26/$J$31)*$M$2</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="L26" s="6">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="M26" s="6" t="e">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
       <c r="N26" s="6" t="e">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>#DIV/0!</v>
       </c>
       <c r="O26" s="8" t="s">
@@ -4995,13 +4995,13 @@
         <v>18</v>
       </c>
       <c r="R26" s="6" t="e">
-        <f>((L26/$L$31)*$P$2)/C26</f>
+        <f t="shared" si="3"/>
         <v>#DIV/0!</v>
       </c>
       <c r="S26" s="2"/>
       <c r="T26" s="7"/>
       <c r="U26" s="17" t="e">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>#DIV/0!</v>
       </c>
       <c r="V26" s="6"/>
@@ -5012,11 +5012,11 @@
         <v>9200</v>
       </c>
       <c r="AA26" s="10" t="e">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>#DIV/0!</v>
       </c>
       <c r="AB26" s="11" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v/>
       </c>
     </row>
@@ -5039,19 +5039,19 @@
         <v>0</v>
       </c>
       <c r="K27" s="6">
-        <f>(J27/$J$31)*$M$2</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="L27" s="6">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="M27" s="6" t="e">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
       <c r="N27" s="6" t="e">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>#DIV/0!</v>
       </c>
       <c r="O27" s="8" t="s">
@@ -5064,13 +5064,13 @@
         <v>18</v>
       </c>
       <c r="R27" s="6" t="e">
-        <f>((L27/$L$31)*$P$2)/C27</f>
+        <f t="shared" si="3"/>
         <v>#DIV/0!</v>
       </c>
       <c r="S27" s="2"/>
       <c r="T27" s="7"/>
       <c r="U27" s="17" t="e">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>#DIV/0!</v>
       </c>
       <c r="V27" s="6"/>
@@ -5081,11 +5081,11 @@
         <v>1300</v>
       </c>
       <c r="AA27" s="10" t="e">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>#DIV/0!</v>
       </c>
       <c r="AB27" s="11" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v/>
       </c>
     </row>
@@ -5108,19 +5108,19 @@
         <v>0</v>
       </c>
       <c r="K28" s="6">
-        <f>(J28/$J$31)*$M$2</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="L28" s="6">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="M28" s="6" t="e">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
       <c r="N28" s="6" t="e">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>#DIV/0!</v>
       </c>
       <c r="O28" s="8" t="s">
@@ -5133,13 +5133,13 @@
         <v>18</v>
       </c>
       <c r="R28" s="6" t="e">
-        <f>((L28/$L$31)*$P$2)/C28</f>
+        <f t="shared" si="3"/>
         <v>#DIV/0!</v>
       </c>
       <c r="S28" s="2"/>
       <c r="T28" s="7"/>
       <c r="U28" s="17" t="e">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>#DIV/0!</v>
       </c>
       <c r="V28" s="6"/>
@@ -5150,11 +5150,11 @@
         <v>1100</v>
       </c>
       <c r="AA28" s="10" t="e">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>#DIV/0!</v>
       </c>
       <c r="AB28" s="11" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v/>
       </c>
     </row>
@@ -5177,19 +5177,19 @@
         <v>0</v>
       </c>
       <c r="K29" s="6">
-        <f>(J29/$J$31)*$M$2</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="L29" s="6">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="M29" s="6" t="e">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
       <c r="N29" s="6" t="e">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>#DIV/0!</v>
       </c>
       <c r="O29" s="8" t="s">
@@ -5202,13 +5202,13 @@
         <v>18</v>
       </c>
       <c r="R29" s="6" t="e">
-        <f>((L29/$L$31)*$P$2)/C29</f>
+        <f t="shared" si="3"/>
         <v>#DIV/0!</v>
       </c>
       <c r="S29" s="2"/>
       <c r="T29" s="7"/>
       <c r="U29" s="17" t="e">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>#DIV/0!</v>
       </c>
       <c r="V29" s="6"/>
@@ -5219,11 +5219,11 @@
         <v>1100</v>
       </c>
       <c r="AA29" s="10" t="e">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>#DIV/0!</v>
       </c>
       <c r="AB29" s="11" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v/>
       </c>
     </row>
@@ -5246,19 +5246,19 @@
         <v>0</v>
       </c>
       <c r="K30" s="6">
-        <f>(J30/$J$31)*$M$2</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="L30" s="6">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="M30" s="6" t="e">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
       <c r="N30" s="6" t="e">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>#DIV/0!</v>
       </c>
       <c r="O30" s="8" t="s">
@@ -5271,13 +5271,13 @@
         <v>18</v>
       </c>
       <c r="R30" s="6" t="e">
-        <f>((L30/$L$31)*$P$2)/C30</f>
+        <f t="shared" si="3"/>
         <v>#DIV/0!</v>
       </c>
       <c r="S30" s="2"/>
       <c r="T30" s="7"/>
       <c r="U30" s="17" t="e">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>#DIV/0!</v>
       </c>
       <c r="V30" s="27"/>
@@ -5288,11 +5288,11 @@
         <v>1700</v>
       </c>
       <c r="AA30" s="10" t="e">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>#DIV/0!</v>
       </c>
       <c r="AB30" s="11" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v/>
       </c>
     </row>

</xml_diff>

<commit_message>
finishing checkout product component
</commit_message>
<xml_diff>
--- a/docs/Costs and pricing-LOCAL.xlsx
+++ b/docs/Costs and pricing-LOCAL.xlsx
@@ -1001,10 +1001,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AB40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B24" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="C1" activePane="topRight" state="frozen"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="M1" activePane="topRight" state="frozen"/>
       <selection activeCell="B1" sqref="B1"/>
-      <selection pane="topRight" activeCell="G25" sqref="G25"/>
+      <selection pane="topRight" activeCell="Y7" sqref="Y7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3313,7 +3313,7 @@
     <sheetView topLeftCell="B1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane xSplit="1" topLeftCell="C1" activePane="topRight" state="frozen"/>
       <selection activeCell="B1" sqref="B1"/>
-      <selection pane="topRight" activeCell="G7" sqref="G7"/>
+      <selection pane="topRight" activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3724,7 +3724,7 @@
         <v>1800</v>
       </c>
       <c r="J8" s="6">
-        <f t="shared" si="0"/>
+        <f>+I8*C8</f>
         <v>18000</v>
       </c>
       <c r="K8" s="6">

</xml_diff>

<commit_message>
adding pages for navs links
</commit_message>
<xml_diff>
--- a/docs/Costs and pricing-LOCAL.xlsx
+++ b/docs/Costs and pricing-LOCAL.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="BOYOUTI" sheetId="1" r:id="rId1"/>
@@ -60,43 +60,8 @@
 </comments>
 </file>
 
-<file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <authors>
-    <author>blida computer</author>
-  </authors>
-  <commentList>
-    <comment ref="B5" authorId="0" shapeId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>blida computer:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-Create a link to the product image 
-put the arrivage in onz folder / supplier</t>
-        </r>
-      </text>
-    </comment>
-  </commentList>
-</comments>
-</file>
-
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="289" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="294" uniqueCount="82">
   <si>
     <t>Markup</t>
   </si>
@@ -305,27 +270,6 @@
     <t>CATEGORY</t>
   </si>
   <si>
-    <t>FITNESS</t>
-  </si>
-  <si>
-    <t>PARFUM</t>
-  </si>
-  <si>
-    <t>FACE CARE</t>
-  </si>
-  <si>
-    <t>BOOTY CARE</t>
-  </si>
-  <si>
-    <t>LIP CARE</t>
-  </si>
-  <si>
-    <t>TEETH CARE</t>
-  </si>
-  <si>
-    <t>BODY CARE</t>
-  </si>
-  <si>
     <t>Guanjing 24K Pure Gold Collagen 30ml</t>
   </si>
   <si>
@@ -338,22 +282,31 @@
     <t>EULMA BUSINESS</t>
   </si>
   <si>
-    <t>DISHWASHING GLOVES</t>
-  </si>
-  <si>
-    <t>HOUSEHOLD</t>
-  </si>
-  <si>
-    <t>MELANGEUR</t>
-  </si>
-  <si>
     <t>SECHOIR</t>
   </si>
   <si>
     <t>BROSSE SECHOIR</t>
   </si>
   <si>
-    <t>HAIRCARE</t>
+    <t>SKINCARE</t>
+  </si>
+  <si>
+    <t>BODY &amp; BATH</t>
+  </si>
+  <si>
+    <t>HAIR</t>
+  </si>
+  <si>
+    <t>PERFUM</t>
+  </si>
+  <si>
+    <t>MAKEUP</t>
+  </si>
+  <si>
+    <t>GIFTS</t>
+  </si>
+  <si>
+    <t>MINI MACHINE A CAFE</t>
   </si>
 </sst>
 </file>
@@ -1001,10 +954,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AB40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="M1" activePane="topRight" state="frozen"/>
+    <sheetView topLeftCell="B27" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="C1" activePane="topRight" state="frozen"/>
       <selection activeCell="B1" sqref="B1"/>
-      <selection pane="topRight" activeCell="Y7" sqref="Y7"/>
+      <selection pane="topRight" activeCell="J32" sqref="J32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1037,12 +990,12 @@
     </row>
     <row r="2" spans="1:28" ht="21" x14ac:dyDescent="0.4">
       <c r="A2" s="21" t="s">
-        <v>77</v>
+        <v>70</v>
       </c>
       <c r="B2" s="22"/>
       <c r="C2" s="34"/>
       <c r="D2" s="22" t="s">
-        <v>78</v>
+        <v>71</v>
       </c>
       <c r="E2" s="16"/>
       <c r="F2" s="16"/>
@@ -1164,13 +1117,13 @@
         <v>1</v>
       </c>
       <c r="B5" s="25" t="s">
-        <v>76</v>
+        <v>69</v>
       </c>
       <c r="C5" s="3">
         <v>12</v>
       </c>
       <c r="D5" s="31" t="s">
-        <v>65</v>
+        <v>75</v>
       </c>
       <c r="E5" s="31"/>
       <c r="F5" s="31"/>
@@ -1186,7 +1139,7 @@
         <v>6000</v>
       </c>
       <c r="K5" s="6">
-        <f t="shared" ref="K5:K31" si="1">(J5/$J$32)*$M$2</f>
+        <f>(J5/$J$32)*$M$2</f>
         <v>29.171194875021449</v>
       </c>
       <c r="L5" s="6">
@@ -1194,7 +1147,7 @@
         <v>6029.1711948750217</v>
       </c>
       <c r="M5" s="6">
-        <f t="shared" ref="M5:M6" si="2">+L5/C5</f>
+        <f t="shared" ref="M5:M6" si="1">+L5/C5</f>
         <v>502.43093290625183</v>
       </c>
       <c r="N5" s="6">
@@ -1230,11 +1183,11 @@
         <v>1400</v>
       </c>
       <c r="AA5" s="10">
-        <f t="shared" ref="AA5:AA31" si="3">(Z5-M5-R5-P5)*C5</f>
+        <f t="shared" ref="AA5:AA31" si="2">(Z5-M5-R5-P5)*C5</f>
         <v>3586.821483727048</v>
       </c>
       <c r="AB5" s="11">
-        <f t="shared" ref="AB5:AB31" si="4">IFERROR(AA5/(M5+P5+R5*C5),"")</f>
+        <f t="shared" ref="AB5:AB31" si="3">IFERROR(AA5/(M5+P5+R5*C5),"")</f>
         <v>1.6404860629684368</v>
       </c>
     </row>
@@ -1249,7 +1202,7 @@
         <v>12</v>
       </c>
       <c r="D6" s="31" t="s">
-        <v>69</v>
+        <v>76</v>
       </c>
       <c r="E6" s="31"/>
       <c r="F6" s="31"/>
@@ -1265,19 +1218,19 @@
         <v>5400</v>
       </c>
       <c r="K6" s="6">
+        <f>(J6/$J$32)*$M$2</f>
+        <v>26.254075387519304</v>
+      </c>
+      <c r="L6" s="6">
+        <f t="shared" ref="L6" si="4">(J6+K6)</f>
+        <v>5426.2540753875192</v>
+      </c>
+      <c r="M6" s="6">
         <f t="shared" si="1"/>
-        <v>26.254075387519304</v>
-      </c>
-      <c r="L6" s="6">
-        <f t="shared" ref="L6" si="5">(J6+K6)</f>
-        <v>5426.2540753875192</v>
-      </c>
-      <c r="M6" s="6">
-        <f t="shared" si="2"/>
         <v>452.18783961562661</v>
       </c>
       <c r="N6" s="6">
-        <f t="shared" ref="N6" si="6">+M6*0.5</f>
+        <f t="shared" ref="N6" si="5">+M6*0.5</f>
         <v>226.09391980781331</v>
       </c>
       <c r="O6" s="8" t="s">
@@ -1290,13 +1243,13 @@
         <v>18</v>
       </c>
       <c r="R6" s="6">
-        <f t="shared" ref="R6:R31" si="7">((L6/$L$32)*$P$2)/C6</f>
+        <f>((L6/$L$32)*$P$2)/C6</f>
         <v>88.800549104844677</v>
       </c>
       <c r="S6" s="2"/>
       <c r="T6" s="7"/>
       <c r="U6" s="17">
-        <f t="shared" ref="U6:U31" si="8">M6+P6+R6+S6+N6</f>
+        <f t="shared" ref="U6:U31" si="6">M6+P6+R6+S6+N6</f>
         <v>1267.0823085282848</v>
       </c>
       <c r="V6" s="6"/>
@@ -1309,11 +1262,11 @@
         <v>1300</v>
       </c>
       <c r="AA6" s="10">
+        <f t="shared" si="2"/>
+        <v>3108.139335354344</v>
+      </c>
+      <c r="AB6" s="11">
         <f t="shared" si="3"/>
-        <v>3108.139335354344</v>
-      </c>
-      <c r="AB6" s="11">
-        <f t="shared" si="4"/>
         <v>1.5403647125188862</v>
       </c>
     </row>
@@ -1328,7 +1281,7 @@
         <v>12</v>
       </c>
       <c r="D7" s="31" t="s">
-        <v>69</v>
+        <v>76</v>
       </c>
       <c r="E7" s="31"/>
       <c r="F7" s="31"/>
@@ -1340,23 +1293,23 @@
         <v>450</v>
       </c>
       <c r="J7" s="6">
-        <f t="shared" ref="J7:J31" si="9">+I7*C7</f>
+        <f t="shared" ref="J7:J31" si="7">+I7*C7</f>
         <v>5400</v>
       </c>
       <c r="K7" s="6">
-        <f t="shared" si="1"/>
+        <f>(J7/$J$32)*$M$2</f>
         <v>26.254075387519304</v>
       </c>
       <c r="L7" s="6">
-        <f t="shared" ref="L7:L31" si="10">(J7+K7)</f>
+        <f t="shared" ref="L7:L31" si="8">(J7+K7)</f>
         <v>5426.2540753875192</v>
       </c>
       <c r="M7" s="6">
-        <f t="shared" ref="M7:M31" si="11">+L7/C7</f>
+        <f t="shared" ref="M7:M31" si="9">+L7/C7</f>
         <v>452.18783961562661</v>
       </c>
       <c r="N7" s="6">
-        <f t="shared" ref="N7:N31" si="12">+M7*0.5</f>
+        <f t="shared" ref="N7:N31" si="10">+M7*0.5</f>
         <v>226.09391980781331</v>
       </c>
       <c r="O7" s="8" t="s">
@@ -1369,13 +1322,13 @@
         <v>18</v>
       </c>
       <c r="R7" s="6">
-        <f t="shared" si="7"/>
+        <f>((L7/$L$32)*$P$2)/C7</f>
         <v>88.800549104844677</v>
       </c>
       <c r="S7" s="2"/>
       <c r="T7" s="7"/>
       <c r="U7" s="17">
-        <f t="shared" si="8"/>
+        <f t="shared" si="6"/>
         <v>1267.0823085282848</v>
       </c>
       <c r="V7" s="6"/>
@@ -1388,11 +1341,11 @@
         <v>1300</v>
       </c>
       <c r="AA7" s="10">
+        <f t="shared" si="2"/>
+        <v>3108.139335354344</v>
+      </c>
+      <c r="AB7" s="11">
         <f t="shared" si="3"/>
-        <v>3108.139335354344</v>
-      </c>
-      <c r="AB7" s="11">
-        <f t="shared" si="4"/>
         <v>1.5403647125188862</v>
       </c>
     </row>
@@ -1407,7 +1360,7 @@
         <v>16</v>
       </c>
       <c r="D8" s="31" t="s">
-        <v>65</v>
+        <v>77</v>
       </c>
       <c r="E8" s="31"/>
       <c r="F8" s="31"/>
@@ -1419,23 +1372,23 @@
         <v>200</v>
       </c>
       <c r="J8" s="6">
+        <f t="shared" si="7"/>
+        <v>3200</v>
+      </c>
+      <c r="K8" s="6">
+        <f>(J8/$J$32)*$M$2</f>
+        <v>15.557970600011439</v>
+      </c>
+      <c r="L8" s="6">
+        <f t="shared" si="8"/>
+        <v>3215.5579706000112</v>
+      </c>
+      <c r="M8" s="6">
         <f t="shared" si="9"/>
-        <v>3200</v>
-      </c>
-      <c r="K8" s="6">
-        <f t="shared" si="1"/>
-        <v>15.557970600011439</v>
-      </c>
-      <c r="L8" s="6">
+        <v>200.9723731625007</v>
+      </c>
+      <c r="N8" s="6">
         <f t="shared" si="10"/>
-        <v>3215.5579706000112</v>
-      </c>
-      <c r="M8" s="6">
-        <f t="shared" si="11"/>
-        <v>200.9723731625007</v>
-      </c>
-      <c r="N8" s="6">
-        <f t="shared" si="12"/>
         <v>100.48618658125035</v>
       </c>
       <c r="O8" s="8" t="s">
@@ -1448,13 +1401,13 @@
         <v>18</v>
       </c>
       <c r="R8" s="6">
-        <f t="shared" si="7"/>
+        <f>((L8/$L$32)*$P$2)/C8</f>
         <v>39.466910713264305</v>
       </c>
       <c r="S8" s="2"/>
       <c r="T8" s="7"/>
       <c r="U8" s="17">
-        <f t="shared" si="8"/>
+        <f t="shared" si="6"/>
         <v>840.92547045701531</v>
       </c>
       <c r="V8" s="6"/>
@@ -1465,11 +1418,11 @@
         <v>900</v>
       </c>
       <c r="AA8" s="10">
+        <f t="shared" si="2"/>
+        <v>2552.97145798776</v>
+      </c>
+      <c r="AB8" s="11">
         <f t="shared" si="3"/>
-        <v>2552.97145798776</v>
-      </c>
-      <c r="AB8" s="11">
-        <f t="shared" si="4"/>
         <v>1.916008087537723</v>
       </c>
     </row>
@@ -1484,7 +1437,7 @@
         <v>2</v>
       </c>
       <c r="D9" s="31" t="s">
-        <v>65</v>
+        <v>75</v>
       </c>
       <c r="E9" s="31"/>
       <c r="F9" s="31" t="s">
@@ -1496,23 +1449,23 @@
         <v>4500</v>
       </c>
       <c r="J9" s="6">
+        <f t="shared" si="7"/>
+        <v>9000</v>
+      </c>
+      <c r="K9" s="6">
+        <f>(J9/$J$32)*$M$2</f>
+        <v>43.756792312532177</v>
+      </c>
+      <c r="L9" s="6">
+        <f t="shared" si="8"/>
+        <v>9043.7567923125316</v>
+      </c>
+      <c r="M9" s="6">
         <f t="shared" si="9"/>
-        <v>9000</v>
-      </c>
-      <c r="K9" s="6">
-        <f t="shared" si="1"/>
-        <v>43.756792312532177</v>
-      </c>
-      <c r="L9" s="6">
+        <v>4521.8783961562658</v>
+      </c>
+      <c r="N9" s="6">
         <f t="shared" si="10"/>
-        <v>9043.7567923125316</v>
-      </c>
-      <c r="M9" s="6">
-        <f t="shared" si="11"/>
-        <v>4521.8783961562658</v>
-      </c>
-      <c r="N9" s="6">
-        <f t="shared" si="12"/>
         <v>2260.9391980781329</v>
       </c>
       <c r="O9" s="8" t="s">
@@ -1525,13 +1478,13 @@
         <v>18</v>
       </c>
       <c r="R9" s="6">
-        <f t="shared" si="7"/>
+        <f>((L9/$L$32)*$P$2)/C9</f>
         <v>888.00549104844686</v>
       </c>
       <c r="S9" s="2"/>
       <c r="T9" s="7"/>
       <c r="U9" s="17">
-        <f t="shared" si="8"/>
+        <f t="shared" si="6"/>
         <v>8170.8230852828456</v>
       </c>
       <c r="V9" s="6"/>
@@ -1544,11 +1497,11 @@
         <v>8500</v>
       </c>
       <c r="AA9" s="10">
+        <f t="shared" si="2"/>
+        <v>5180.2322255905747</v>
+      </c>
+      <c r="AB9" s="11">
         <f t="shared" si="3"/>
-        <v>5180.2322255905747</v>
-      </c>
-      <c r="AB9" s="11">
-        <f t="shared" si="4"/>
         <v>0.76203538147626182</v>
       </c>
     </row>
@@ -1563,7 +1516,7 @@
         <v>20</v>
       </c>
       <c r="D10" s="31" t="s">
-        <v>70</v>
+        <v>78</v>
       </c>
       <c r="E10" s="31"/>
       <c r="F10" s="31"/>
@@ -1575,23 +1528,23 @@
         <v>450</v>
       </c>
       <c r="J10" s="6">
+        <f t="shared" si="7"/>
+        <v>9000</v>
+      </c>
+      <c r="K10" s="6">
+        <f>(J10/$J$32)*$M$2</f>
+        <v>43.756792312532177</v>
+      </c>
+      <c r="L10" s="6">
+        <f t="shared" si="8"/>
+        <v>9043.7567923125316</v>
+      </c>
+      <c r="M10" s="6">
         <f t="shared" si="9"/>
-        <v>9000</v>
-      </c>
-      <c r="K10" s="6">
-        <f t="shared" si="1"/>
-        <v>43.756792312532177</v>
-      </c>
-      <c r="L10" s="6">
+        <v>452.18783961562656</v>
+      </c>
+      <c r="N10" s="6">
         <f t="shared" si="10"/>
-        <v>9043.7567923125316</v>
-      </c>
-      <c r="M10" s="6">
-        <f t="shared" si="11"/>
-        <v>452.18783961562656</v>
-      </c>
-      <c r="N10" s="6">
-        <f t="shared" si="12"/>
         <v>226.09391980781328</v>
       </c>
       <c r="O10" s="8" t="s">
@@ -1604,13 +1557,13 @@
         <v>18</v>
       </c>
       <c r="R10" s="6">
-        <f t="shared" si="7"/>
+        <f>((L10/$L$32)*$P$2)/C10</f>
         <v>88.800549104844691</v>
       </c>
       <c r="S10" s="2"/>
       <c r="T10" s="7"/>
       <c r="U10" s="17">
-        <f t="shared" si="8"/>
+        <f t="shared" si="6"/>
         <v>1267.0823085282846</v>
       </c>
       <c r="V10" s="6"/>
@@ -1621,11 +1574,11 @@
         <v>1400</v>
       </c>
       <c r="AA10" s="10">
+        <f t="shared" si="2"/>
+        <v>7180.2322255905756</v>
+      </c>
+      <c r="AB10" s="11">
         <f t="shared" si="3"/>
-        <v>7180.2322255905756</v>
-      </c>
-      <c r="AB10" s="11">
-        <f t="shared" si="4"/>
         <v>2.6318581213532908</v>
       </c>
     </row>
@@ -1640,7 +1593,7 @@
         <v>12</v>
       </c>
       <c r="D11" s="31" t="s">
-        <v>71</v>
+        <v>75</v>
       </c>
       <c r="E11" s="31"/>
       <c r="F11" s="31"/>
@@ -1652,23 +1605,23 @@
         <v>300</v>
       </c>
       <c r="J11" s="6">
+        <f t="shared" si="7"/>
+        <v>3600</v>
+      </c>
+      <c r="K11" s="6">
+        <f>(J11/$J$32)*$M$2</f>
+        <v>17.502716925012869</v>
+      </c>
+      <c r="L11" s="6">
+        <f t="shared" si="8"/>
+        <v>3617.5027169250129</v>
+      </c>
+      <c r="M11" s="6">
         <f t="shared" si="9"/>
-        <v>3600</v>
-      </c>
-      <c r="K11" s="6">
-        <f t="shared" si="1"/>
-        <v>17.502716925012869</v>
-      </c>
-      <c r="L11" s="6">
+        <v>301.4585597437511</v>
+      </c>
+      <c r="N11" s="6">
         <f t="shared" si="10"/>
-        <v>3617.5027169250129</v>
-      </c>
-      <c r="M11" s="6">
-        <f t="shared" si="11"/>
-        <v>301.4585597437511</v>
-      </c>
-      <c r="N11" s="6">
-        <f t="shared" si="12"/>
         <v>150.72927987187555</v>
       </c>
       <c r="O11" s="8" t="s">
@@ -1681,13 +1634,13 @@
         <v>18</v>
       </c>
       <c r="R11" s="6">
-        <f t="shared" si="7"/>
+        <f>((L11/$L$32)*$P$2)/C11</f>
         <v>59.200366069896461</v>
       </c>
       <c r="S11" s="2"/>
       <c r="T11" s="7"/>
       <c r="U11" s="17">
-        <f t="shared" si="8"/>
+        <f t="shared" si="6"/>
         <v>1011.3882056855231</v>
       </c>
       <c r="V11" s="6"/>
@@ -1698,11 +1651,11 @@
         <v>1100</v>
       </c>
       <c r="AA11" s="10">
+        <f t="shared" si="2"/>
+        <v>2872.0928902362293</v>
+      </c>
+      <c r="AB11" s="11">
         <f t="shared" si="3"/>
-        <v>2872.0928902362293</v>
-      </c>
-      <c r="AB11" s="11">
-        <f t="shared" si="4"/>
         <v>1.8997045237005286</v>
       </c>
     </row>
@@ -1717,7 +1670,7 @@
         <v>4</v>
       </c>
       <c r="D12" s="31" t="s">
-        <v>72</v>
+        <v>76</v>
       </c>
       <c r="E12" s="31"/>
       <c r="F12" s="31"/>
@@ -1729,23 +1682,23 @@
         <v>370</v>
       </c>
       <c r="J12" s="6">
+        <f t="shared" si="7"/>
+        <v>1480</v>
+      </c>
+      <c r="K12" s="6">
+        <f>(J12/$J$32)*$M$2</f>
+        <v>7.195561402505291</v>
+      </c>
+      <c r="L12" s="6">
+        <f t="shared" si="8"/>
+        <v>1487.1955614025053</v>
+      </c>
+      <c r="M12" s="6">
         <f t="shared" si="9"/>
-        <v>1480</v>
-      </c>
-      <c r="K12" s="6">
-        <f t="shared" si="1"/>
-        <v>7.195561402505291</v>
-      </c>
-      <c r="L12" s="6">
+        <v>371.79889035062632</v>
+      </c>
+      <c r="N12" s="6">
         <f t="shared" si="10"/>
-        <v>1487.1955614025053</v>
-      </c>
-      <c r="M12" s="6">
-        <f t="shared" si="11"/>
-        <v>371.79889035062632</v>
-      </c>
-      <c r="N12" s="6">
-        <f t="shared" si="12"/>
         <v>185.89944517531316</v>
       </c>
       <c r="O12" s="8" t="s">
@@ -1758,13 +1711,13 @@
         <v>18</v>
       </c>
       <c r="R12" s="6">
-        <f t="shared" si="7"/>
+        <f>((L12/$L$32)*$P$2)/C12</f>
         <v>73.013784819538969</v>
       </c>
       <c r="S12" s="2"/>
       <c r="T12" s="7"/>
       <c r="U12" s="17">
-        <f t="shared" si="8"/>
+        <f t="shared" si="6"/>
         <v>1130.7121203454785</v>
       </c>
       <c r="V12" s="6"/>
@@ -1775,11 +1728,11 @@
         <v>1200</v>
       </c>
       <c r="AA12" s="10">
+        <f t="shared" si="2"/>
+        <v>1020.7492993193387</v>
+      </c>
+      <c r="AB12" s="11">
         <f t="shared" si="3"/>
-        <v>1020.7492993193387</v>
-      </c>
-      <c r="AB12" s="11">
-        <f t="shared" si="4"/>
         <v>0.87704237243987748</v>
       </c>
     </row>
@@ -1794,7 +1747,7 @@
         <v>4</v>
       </c>
       <c r="D13" s="31" t="s">
-        <v>72</v>
+        <v>76</v>
       </c>
       <c r="E13" s="31"/>
       <c r="F13" s="31"/>
@@ -1804,23 +1757,23 @@
         <v>470</v>
       </c>
       <c r="J13" s="6">
+        <f t="shared" si="7"/>
+        <v>1880</v>
+      </c>
+      <c r="K13" s="6">
+        <f>(J13/$J$32)*$M$2</f>
+        <v>9.1403077275067215</v>
+      </c>
+      <c r="L13" s="6">
+        <f t="shared" si="8"/>
+        <v>1889.1403077275068</v>
+      </c>
+      <c r="M13" s="6">
         <f t="shared" si="9"/>
-        <v>1880</v>
-      </c>
-      <c r="K13" s="6">
-        <f t="shared" si="1"/>
-        <v>9.1403077275067215</v>
-      </c>
-      <c r="L13" s="6">
+        <v>472.28507693187669</v>
+      </c>
+      <c r="N13" s="6">
         <f t="shared" si="10"/>
-        <v>1889.1403077275068</v>
-      </c>
-      <c r="M13" s="6">
-        <f t="shared" si="11"/>
-        <v>472.28507693187669</v>
-      </c>
-      <c r="N13" s="6">
-        <f t="shared" si="12"/>
         <v>236.14253846593834</v>
       </c>
       <c r="O13" s="8" t="s">
@@ -1833,13 +1786,13 @@
         <v>18</v>
       </c>
       <c r="R13" s="6">
-        <f t="shared" si="7"/>
+        <f>((L13/$L$32)*$P$2)/C13</f>
         <v>92.747240176171132</v>
       </c>
       <c r="S13" s="2"/>
       <c r="T13" s="7"/>
       <c r="U13" s="17">
-        <f t="shared" si="8"/>
+        <f t="shared" si="6"/>
         <v>1301.1748555739862</v>
       </c>
       <c r="V13" s="6"/>
@@ -1850,11 +1803,11 @@
         <v>1350</v>
       </c>
       <c r="AA13" s="10">
+        <f t="shared" si="2"/>
+        <v>1139.8707315678089</v>
+      </c>
+      <c r="AB13" s="11">
         <f t="shared" si="3"/>
-        <v>1139.8707315678089</v>
-      </c>
-      <c r="AB13" s="11">
-        <f t="shared" si="4"/>
         <v>0.84857646290355426</v>
       </c>
     </row>
@@ -1869,7 +1822,7 @@
         <v>11</v>
       </c>
       <c r="D14" s="31" t="s">
-        <v>73</v>
+        <v>79</v>
       </c>
       <c r="E14" s="31"/>
       <c r="F14" s="31"/>
@@ -1881,23 +1834,23 @@
         <v>700</v>
       </c>
       <c r="J14" s="6">
+        <f t="shared" si="7"/>
+        <v>7700</v>
+      </c>
+      <c r="K14" s="6">
+        <f>(J14/$J$32)*$M$2</f>
+        <v>37.436366756277522</v>
+      </c>
+      <c r="L14" s="6">
+        <f t="shared" si="8"/>
+        <v>7737.4363667562775</v>
+      </c>
+      <c r="M14" s="6">
         <f t="shared" si="9"/>
-        <v>7700</v>
-      </c>
-      <c r="K14" s="6">
-        <f t="shared" si="1"/>
-        <v>37.436366756277522</v>
-      </c>
-      <c r="L14" s="6">
+        <v>703.4033060687525</v>
+      </c>
+      <c r="N14" s="6">
         <f t="shared" si="10"/>
-        <v>7737.4363667562775</v>
-      </c>
-      <c r="M14" s="6">
-        <f t="shared" si="11"/>
-        <v>703.4033060687525</v>
-      </c>
-      <c r="N14" s="6">
-        <f t="shared" si="12"/>
         <v>351.70165303437625</v>
       </c>
       <c r="O14" s="8" t="s">
@@ -1910,13 +1863,13 @@
         <v>18</v>
       </c>
       <c r="R14" s="6">
-        <f t="shared" si="7"/>
+        <f>((L14/$L$32)*$P$2)/C14</f>
         <v>138.13418749642508</v>
       </c>
       <c r="S14" s="2"/>
       <c r="T14" s="7"/>
       <c r="U14" s="17">
-        <f t="shared" si="8"/>
+        <f t="shared" si="6"/>
         <v>1693.2391465995538</v>
       </c>
       <c r="V14" s="6"/>
@@ -1927,11 +1880,11 @@
         <v>1700</v>
       </c>
       <c r="AA14" s="10">
+        <f t="shared" si="2"/>
+        <v>3943.0875707830469</v>
+      </c>
+      <c r="AB14" s="11">
         <f t="shared" si="3"/>
-        <v>3943.0875707830469</v>
-      </c>
-      <c r="AB14" s="11">
-        <f t="shared" si="4"/>
         <v>1.4481315684993521</v>
       </c>
     </row>
@@ -1946,7 +1899,7 @@
         <v>55</v>
       </c>
       <c r="D15" s="31" t="s">
-        <v>73</v>
+        <v>79</v>
       </c>
       <c r="E15" s="31"/>
       <c r="F15" s="31"/>
@@ -1958,23 +1911,23 @@
         <v>800</v>
       </c>
       <c r="J15" s="6">
+        <f t="shared" si="7"/>
+        <v>44000</v>
+      </c>
+      <c r="K15" s="6">
+        <f>(J15/$J$32)*$M$2</f>
+        <v>213.9220957501573</v>
+      </c>
+      <c r="L15" s="6">
+        <f t="shared" si="8"/>
+        <v>44213.92209575016</v>
+      </c>
+      <c r="M15" s="6">
         <f t="shared" si="9"/>
-        <v>44000</v>
-      </c>
-      <c r="K15" s="6">
-        <f t="shared" si="1"/>
-        <v>213.9220957501573</v>
-      </c>
-      <c r="L15" s="6">
+        <v>803.88949265000292</v>
+      </c>
+      <c r="N15" s="6">
         <f t="shared" si="10"/>
-        <v>44213.92209575016</v>
-      </c>
-      <c r="M15" s="6">
-        <f t="shared" si="11"/>
-        <v>803.88949265000292</v>
-      </c>
-      <c r="N15" s="6">
-        <f t="shared" si="12"/>
         <v>401.94474632500146</v>
       </c>
       <c r="O15" s="8" t="s">
@@ -1987,13 +1940,13 @@
         <v>18</v>
       </c>
       <c r="R15" s="6">
-        <f t="shared" si="7"/>
+        <f>((L15/$L$32)*$P$2)/C15</f>
         <v>157.86764285305725</v>
       </c>
       <c r="S15" s="2"/>
       <c r="T15" s="7"/>
       <c r="U15" s="17">
-        <f t="shared" si="8"/>
+        <f t="shared" si="6"/>
         <v>1863.7018818280617</v>
       </c>
       <c r="V15" s="6"/>
@@ -2004,11 +1957,11 @@
         <v>1900</v>
       </c>
       <c r="AA15" s="10">
+        <f t="shared" si="2"/>
+        <v>24103.357547331689</v>
+      </c>
+      <c r="AB15" s="11">
         <f t="shared" si="3"/>
-        <v>24103.357547331689</v>
-      </c>
-      <c r="AB15" s="11">
-        <f t="shared" si="4"/>
         <v>2.4135675580010751</v>
       </c>
     </row>
@@ -2023,7 +1976,7 @@
         <v>12</v>
       </c>
       <c r="D16" s="31" t="s">
-        <v>65</v>
+        <v>75</v>
       </c>
       <c r="E16" s="31"/>
       <c r="F16" s="31"/>
@@ -2035,23 +1988,23 @@
         <v>750</v>
       </c>
       <c r="J16" s="6">
+        <f t="shared" si="7"/>
+        <v>9000</v>
+      </c>
+      <c r="K16" s="6">
+        <f>(J16/$J$32)*$M$2</f>
+        <v>43.756792312532177</v>
+      </c>
+      <c r="L16" s="6">
+        <f t="shared" si="8"/>
+        <v>9043.7567923125316</v>
+      </c>
+      <c r="M16" s="6">
         <f t="shared" si="9"/>
-        <v>9000</v>
-      </c>
-      <c r="K16" s="6">
-        <f t="shared" si="1"/>
-        <v>43.756792312532177</v>
-      </c>
-      <c r="L16" s="6">
+        <v>753.6463993593776</v>
+      </c>
+      <c r="N16" s="6">
         <f t="shared" si="10"/>
-        <v>9043.7567923125316</v>
-      </c>
-      <c r="M16" s="6">
-        <f t="shared" si="11"/>
-        <v>753.6463993593776</v>
-      </c>
-      <c r="N16" s="6">
-        <f t="shared" si="12"/>
         <v>376.8231996796888</v>
       </c>
       <c r="O16" s="8" t="s">
@@ -2064,13 +2017,13 @@
         <v>18</v>
       </c>
       <c r="R16" s="6">
-        <f t="shared" si="7"/>
+        <f>((L16/$L$32)*$P$2)/C16</f>
         <v>148.00091517474115</v>
       </c>
       <c r="S16" s="2"/>
       <c r="T16" s="7"/>
       <c r="U16" s="17">
-        <f t="shared" si="8"/>
+        <f t="shared" si="6"/>
         <v>1778.4705142138073</v>
       </c>
       <c r="V16" s="6"/>
@@ -2081,11 +2034,11 @@
         <v>1800</v>
       </c>
       <c r="AA16" s="10">
+        <f t="shared" si="2"/>
+        <v>4780.2322255905765</v>
+      </c>
+      <c r="AB16" s="11">
         <f t="shared" si="3"/>
-        <v>4780.2322255905765</v>
-      </c>
-      <c r="AB16" s="11">
-        <f t="shared" si="4"/>
         <v>1.577812809741824</v>
       </c>
     </row>
@@ -2100,7 +2053,7 @@
         <v>24</v>
       </c>
       <c r="D17" s="31" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="E17" s="31"/>
       <c r="F17" s="31"/>
@@ -2112,23 +2065,23 @@
         <v>1200</v>
       </c>
       <c r="J17" s="6">
+        <f t="shared" si="7"/>
+        <v>28800</v>
+      </c>
+      <c r="K17" s="6">
+        <f>(J17/$J$32)*$M$2</f>
+        <v>140.02173540010295</v>
+      </c>
+      <c r="L17" s="6">
+        <f t="shared" si="8"/>
+        <v>28940.021735400103</v>
+      </c>
+      <c r="M17" s="6">
         <f t="shared" si="9"/>
-        <v>28800</v>
-      </c>
-      <c r="K17" s="6">
-        <f t="shared" si="1"/>
-        <v>140.02173540010295</v>
-      </c>
-      <c r="L17" s="6">
+        <v>1205.8342389750044</v>
+      </c>
+      <c r="N17" s="6">
         <f t="shared" si="10"/>
-        <v>28940.021735400103</v>
-      </c>
-      <c r="M17" s="6">
-        <f t="shared" si="11"/>
-        <v>1205.8342389750044</v>
-      </c>
-      <c r="N17" s="6">
-        <f t="shared" si="12"/>
         <v>602.91711948750219</v>
       </c>
       <c r="O17" s="8" t="s">
@@ -2141,13 +2094,13 @@
         <v>18</v>
       </c>
       <c r="R17" s="6">
-        <f t="shared" si="7"/>
+        <f>((L17/$L$32)*$P$2)/C17</f>
         <v>236.80146427958584</v>
       </c>
       <c r="S17" s="2"/>
       <c r="T17" s="7"/>
       <c r="U17" s="17">
-        <f t="shared" si="8"/>
+        <f t="shared" si="6"/>
         <v>2545.5528227420923</v>
       </c>
       <c r="V17" s="6"/>
@@ -2158,11 +2111,11 @@
         <v>2600</v>
       </c>
       <c r="AA17" s="10">
+        <f t="shared" si="2"/>
+        <v>15776.743121889835</v>
+      </c>
+      <c r="AB17" s="11">
         <f t="shared" si="3"/>
-        <v>15776.743121889835</v>
-      </c>
-      <c r="AB17" s="11">
-        <f t="shared" si="4"/>
         <v>2.1351461607594184</v>
       </c>
     </row>
@@ -2189,23 +2142,23 @@
         <v>350</v>
       </c>
       <c r="J18" s="6">
+        <f t="shared" si="7"/>
+        <v>8400</v>
+      </c>
+      <c r="K18" s="6">
+        <f>(J18/$J$32)*$M$2</f>
+        <v>40.839672825030028</v>
+      </c>
+      <c r="L18" s="6">
+        <f t="shared" si="8"/>
+        <v>8440.83967282503</v>
+      </c>
+      <c r="M18" s="6">
         <f t="shared" si="9"/>
-        <v>8400</v>
-      </c>
-      <c r="K18" s="6">
-        <f t="shared" si="1"/>
-        <v>40.839672825030028</v>
-      </c>
-      <c r="L18" s="6">
+        <v>351.70165303437625</v>
+      </c>
+      <c r="N18" s="6">
         <f t="shared" si="10"/>
-        <v>8440.83967282503</v>
-      </c>
-      <c r="M18" s="6">
-        <f t="shared" si="11"/>
-        <v>351.70165303437625</v>
-      </c>
-      <c r="N18" s="6">
-        <f t="shared" si="12"/>
         <v>175.85082651718812</v>
       </c>
       <c r="O18" s="8" t="s">
@@ -2218,13 +2171,13 @@
         <v>18</v>
       </c>
       <c r="R18" s="6">
-        <f t="shared" si="7"/>
+        <f>((L18/$L$32)*$P$2)/C18</f>
         <v>69.067093748212542</v>
       </c>
       <c r="S18" s="2"/>
       <c r="T18" s="7"/>
       <c r="U18" s="17">
-        <f t="shared" si="8"/>
+        <f t="shared" si="6"/>
         <v>1096.6195732997769</v>
       </c>
       <c r="V18" s="6"/>
@@ -2235,11 +2188,11 @@
         <v>1100</v>
       </c>
       <c r="AA18" s="10">
+        <f t="shared" si="2"/>
+        <v>4301.5500772178693</v>
+      </c>
+      <c r="AB18" s="11">
         <f t="shared" si="3"/>
-        <v>4301.5500772178693</v>
-      </c>
-      <c r="AB18" s="11">
-        <f t="shared" si="4"/>
         <v>1.7142349151931948</v>
       </c>
     </row>
@@ -2253,7 +2206,9 @@
       <c r="C19" s="3">
         <v>20</v>
       </c>
-      <c r="D19" s="31"/>
+      <c r="D19" s="31" t="s">
+        <v>75</v>
+      </c>
       <c r="E19" s="31"/>
       <c r="F19" s="31"/>
       <c r="G19" s="31"/>
@@ -2264,23 +2219,23 @@
         <v>1050</v>
       </c>
       <c r="J19" s="6">
+        <f t="shared" si="7"/>
+        <v>21000</v>
+      </c>
+      <c r="K19" s="6">
+        <f>(J19/$J$32)*$M$2</f>
+        <v>102.09918206257508</v>
+      </c>
+      <c r="L19" s="6">
+        <f t="shared" si="8"/>
+        <v>21102.099182062575</v>
+      </c>
+      <c r="M19" s="6">
         <f t="shared" si="9"/>
-        <v>21000</v>
-      </c>
-      <c r="K19" s="6">
-        <f t="shared" si="1"/>
-        <v>102.09918206257508</v>
-      </c>
-      <c r="L19" s="6">
+        <v>1055.1049591031287</v>
+      </c>
+      <c r="N19" s="6">
         <f t="shared" si="10"/>
-        <v>21102.099182062575</v>
-      </c>
-      <c r="M19" s="6">
-        <f t="shared" si="11"/>
-        <v>1055.1049591031287</v>
-      </c>
-      <c r="N19" s="6">
-        <f t="shared" si="12"/>
         <v>527.55247955156437</v>
       </c>
       <c r="O19" s="8" t="s">
@@ -2293,13 +2248,13 @@
         <v>18</v>
       </c>
       <c r="R19" s="6">
-        <f t="shared" si="7"/>
+        <f>((L19/$L$32)*$P$2)/C19</f>
         <v>207.20128124463764</v>
       </c>
       <c r="S19" s="2"/>
       <c r="T19" s="7"/>
       <c r="U19" s="17">
-        <f t="shared" si="8"/>
+        <f t="shared" si="6"/>
         <v>2289.8587198993309</v>
       </c>
       <c r="V19" s="6"/>
@@ -2310,11 +2265,11 @@
         <v>2300</v>
       </c>
       <c r="AA19" s="10">
+        <f t="shared" si="2"/>
+        <v>10753.875193044674</v>
+      </c>
+      <c r="AB19" s="11">
         <f t="shared" si="3"/>
-        <v>10753.875193044674</v>
-      </c>
-      <c r="AB19" s="11">
-        <f t="shared" si="4"/>
         <v>1.8869325828826184</v>
       </c>
     </row>
@@ -2328,7 +2283,9 @@
       <c r="C20" s="3">
         <v>12</v>
       </c>
-      <c r="D20" s="31"/>
+      <c r="D20" s="31" t="s">
+        <v>75</v>
+      </c>
       <c r="E20" s="31"/>
       <c r="F20" s="31"/>
       <c r="G20" s="31"/>
@@ -2339,23 +2296,23 @@
         <v>350</v>
       </c>
       <c r="J20" s="6">
+        <f t="shared" si="7"/>
+        <v>4200</v>
+      </c>
+      <c r="K20" s="6">
+        <f>(J20/$J$32)*$M$2</f>
+        <v>20.419836412515014</v>
+      </c>
+      <c r="L20" s="6">
+        <f t="shared" si="8"/>
+        <v>4220.419836412515</v>
+      </c>
+      <c r="M20" s="6">
         <f t="shared" si="9"/>
-        <v>4200</v>
-      </c>
-      <c r="K20" s="6">
-        <f t="shared" si="1"/>
-        <v>20.419836412515014</v>
-      </c>
-      <c r="L20" s="6">
+        <v>351.70165303437625</v>
+      </c>
+      <c r="N20" s="6">
         <f t="shared" si="10"/>
-        <v>4220.419836412515</v>
-      </c>
-      <c r="M20" s="6">
-        <f t="shared" si="11"/>
-        <v>351.70165303437625</v>
-      </c>
-      <c r="N20" s="6">
-        <f t="shared" si="12"/>
         <v>175.85082651718812</v>
       </c>
       <c r="O20" s="8" t="s">
@@ -2368,13 +2325,13 @@
         <v>18</v>
       </c>
       <c r="R20" s="6">
-        <f t="shared" si="7"/>
+        <f>((L20/$L$32)*$P$2)/C20</f>
         <v>69.067093748212542</v>
       </c>
       <c r="S20" s="2"/>
       <c r="T20" s="7"/>
       <c r="U20" s="17">
-        <f t="shared" si="8"/>
+        <f t="shared" si="6"/>
         <v>1096.6195732997769</v>
       </c>
       <c r="V20" s="6"/>
@@ -2385,11 +2342,11 @@
         <v>1100</v>
       </c>
       <c r="AA20" s="10">
+        <f t="shared" si="2"/>
+        <v>2150.7750386089347</v>
+      </c>
+      <c r="AB20" s="11">
         <f t="shared" si="3"/>
-        <v>2150.7750386089347</v>
-      </c>
-      <c r="AB20" s="11">
-        <f t="shared" si="4"/>
         <v>1.2798371698042568</v>
       </c>
     </row>
@@ -2403,7 +2360,9 @@
       <c r="C21" s="3">
         <v>48</v>
       </c>
-      <c r="D21" s="31"/>
+      <c r="D21" s="31" t="s">
+        <v>79</v>
+      </c>
       <c r="E21" s="31"/>
       <c r="F21" s="31"/>
       <c r="G21" s="31"/>
@@ -2414,23 +2373,23 @@
         <v>95</v>
       </c>
       <c r="J21" s="6">
+        <f t="shared" si="7"/>
+        <v>4560</v>
+      </c>
+      <c r="K21" s="6">
+        <f>(J21/$J$32)*$M$2</f>
+        <v>22.1701081050163</v>
+      </c>
+      <c r="L21" s="6">
+        <f t="shared" si="8"/>
+        <v>4582.170108105016</v>
+      </c>
+      <c r="M21" s="6">
         <f t="shared" si="9"/>
-        <v>4560</v>
-      </c>
-      <c r="K21" s="6">
-        <f t="shared" si="1"/>
-        <v>22.1701081050163</v>
-      </c>
-      <c r="L21" s="6">
+        <v>95.461877252187833</v>
+      </c>
+      <c r="N21" s="6">
         <f t="shared" si="10"/>
-        <v>4582.170108105016</v>
-      </c>
-      <c r="M21" s="6">
-        <f t="shared" si="11"/>
-        <v>95.461877252187833</v>
-      </c>
-      <c r="N21" s="6">
-        <f t="shared" si="12"/>
         <v>47.730938626093916</v>
       </c>
       <c r="O21" s="8" t="s">
@@ -2443,13 +2402,13 @@
         <v>18</v>
       </c>
       <c r="R21" s="6">
-        <f t="shared" si="7"/>
+        <f>((L21/$L$32)*$P$2)/C21</f>
         <v>18.746782588800546</v>
       </c>
       <c r="S21" s="2"/>
       <c r="T21" s="7"/>
       <c r="U21" s="17">
-        <f t="shared" si="8"/>
+        <f t="shared" si="6"/>
         <v>661.93959846708231</v>
       </c>
       <c r="V21" s="6"/>
@@ -2460,11 +2419,11 @@
         <v>700</v>
       </c>
       <c r="AA21" s="10">
+        <f t="shared" si="2"/>
+        <v>4117.9843276325573</v>
+      </c>
+      <c r="AB21" s="11">
         <f t="shared" si="3"/>
-        <v>4117.9843276325573</v>
-      </c>
-      <c r="AB21" s="11">
-        <f t="shared" si="4"/>
         <v>2.7539382292255588</v>
       </c>
     </row>
@@ -2478,7 +2437,9 @@
       <c r="C22" s="3">
         <v>144</v>
       </c>
-      <c r="D22" s="31"/>
+      <c r="D22" s="31" t="s">
+        <v>75</v>
+      </c>
       <c r="E22" s="31"/>
       <c r="F22" s="31"/>
       <c r="G22" s="31"/>
@@ -2489,23 +2450,23 @@
         <v>150</v>
       </c>
       <c r="J22" s="6">
+        <f t="shared" si="7"/>
+        <v>21600</v>
+      </c>
+      <c r="K22" s="6">
+        <f>(J22/$J$32)*$M$2</f>
+        <v>105.01630155007722</v>
+      </c>
+      <c r="L22" s="6">
+        <f t="shared" si="8"/>
+        <v>21705.016301550077</v>
+      </c>
+      <c r="M22" s="6">
         <f t="shared" si="9"/>
-        <v>21600</v>
-      </c>
-      <c r="K22" s="6">
-        <f t="shared" si="1"/>
-        <v>105.01630155007722</v>
-      </c>
-      <c r="L22" s="6">
+        <v>150.72927987187552</v>
+      </c>
+      <c r="N22" s="6">
         <f t="shared" si="10"/>
-        <v>21705.016301550077</v>
-      </c>
-      <c r="M22" s="6">
-        <f t="shared" si="11"/>
-        <v>150.72927987187552</v>
-      </c>
-      <c r="N22" s="6">
-        <f t="shared" si="12"/>
         <v>75.36463993593776</v>
       </c>
       <c r="O22" s="8" t="s">
@@ -2518,13 +2479,13 @@
         <v>18</v>
       </c>
       <c r="R22" s="6">
-        <f t="shared" si="7"/>
+        <f>((L22/$L$32)*$P$2)/C22</f>
         <v>29.600183034948227</v>
       </c>
       <c r="S22" s="2"/>
       <c r="T22" s="7"/>
       <c r="U22" s="17">
-        <f t="shared" si="8"/>
+        <f t="shared" si="6"/>
         <v>755.69410284276159</v>
       </c>
       <c r="V22" s="6"/>
@@ -2535,11 +2496,11 @@
         <v>800</v>
       </c>
       <c r="AA22" s="10">
+        <f t="shared" si="2"/>
+        <v>17232.557341417378</v>
+      </c>
+      <c r="AB22" s="11">
         <f t="shared" si="3"/>
-        <v>17232.557341417378</v>
-      </c>
-      <c r="AB22" s="11">
-        <f t="shared" si="4"/>
         <v>3.5074316009811795</v>
       </c>
     </row>
@@ -2553,7 +2514,9 @@
       <c r="C23" s="3">
         <v>24</v>
       </c>
-      <c r="D23" s="31"/>
+      <c r="D23" s="31" t="s">
+        <v>75</v>
+      </c>
       <c r="E23" s="31"/>
       <c r="F23" s="31"/>
       <c r="G23" s="31"/>
@@ -2564,23 +2527,23 @@
         <v>160</v>
       </c>
       <c r="J23" s="6">
+        <f t="shared" si="7"/>
+        <v>3840</v>
+      </c>
+      <c r="K23" s="6">
+        <f>(J23/$J$32)*$M$2</f>
+        <v>18.669564720013728</v>
+      </c>
+      <c r="L23" s="6">
+        <f t="shared" si="8"/>
+        <v>3858.6695647200136</v>
+      </c>
+      <c r="M23" s="6">
         <f t="shared" si="9"/>
-        <v>3840</v>
-      </c>
-      <c r="K23" s="6">
-        <f t="shared" si="1"/>
-        <v>18.669564720013728</v>
-      </c>
-      <c r="L23" s="6">
+        <v>160.77789853000056</v>
+      </c>
+      <c r="N23" s="6">
         <f t="shared" si="10"/>
-        <v>3858.6695647200136</v>
-      </c>
-      <c r="M23" s="6">
-        <f t="shared" si="11"/>
-        <v>160.77789853000056</v>
-      </c>
-      <c r="N23" s="6">
-        <f t="shared" si="12"/>
         <v>80.388949265000278</v>
       </c>
       <c r="O23" s="8" t="s">
@@ -2593,13 +2556,13 @@
         <v>18</v>
       </c>
       <c r="R23" s="6">
-        <f t="shared" si="7"/>
+        <f>((L23/$L$32)*$P$2)/C23</f>
         <v>31.573528570611444</v>
       </c>
       <c r="S23" s="2"/>
       <c r="T23" s="7"/>
       <c r="U23" s="17">
-        <f t="shared" si="8"/>
+        <f t="shared" si="6"/>
         <v>772.74037636561229</v>
       </c>
       <c r="V23" s="6"/>
@@ -2610,11 +2573,11 @@
         <v>800</v>
       </c>
       <c r="AA23" s="10">
+        <f t="shared" si="2"/>
+        <v>2583.565749585312</v>
+      </c>
+      <c r="AB23" s="11">
         <f t="shared" si="3"/>
-        <v>2583.565749585312</v>
-      </c>
-      <c r="AB23" s="11">
-        <f t="shared" si="4"/>
         <v>1.8212817706825466</v>
       </c>
     </row>
@@ -2628,7 +2591,9 @@
       <c r="C24" s="3">
         <v>16</v>
       </c>
-      <c r="D24" s="31"/>
+      <c r="D24" s="31" t="s">
+        <v>79</v>
+      </c>
       <c r="E24" s="31"/>
       <c r="F24" s="31"/>
       <c r="G24" s="31"/>
@@ -2639,23 +2604,23 @@
         <v>350</v>
       </c>
       <c r="J24" s="6">
+        <f t="shared" si="7"/>
+        <v>5600</v>
+      </c>
+      <c r="K24" s="6">
+        <f>(J24/$J$32)*$M$2</f>
+        <v>27.226448550020017</v>
+      </c>
+      <c r="L24" s="6">
+        <f t="shared" si="8"/>
+        <v>5627.22644855002</v>
+      </c>
+      <c r="M24" s="6">
         <f t="shared" si="9"/>
-        <v>5600</v>
-      </c>
-      <c r="K24" s="6">
-        <f t="shared" si="1"/>
-        <v>27.226448550020017</v>
-      </c>
-      <c r="L24" s="6">
+        <v>351.70165303437625</v>
+      </c>
+      <c r="N24" s="6">
         <f t="shared" si="10"/>
-        <v>5627.22644855002</v>
-      </c>
-      <c r="M24" s="6">
-        <f t="shared" si="11"/>
-        <v>351.70165303437625</v>
-      </c>
-      <c r="N24" s="6">
-        <f t="shared" si="12"/>
         <v>175.85082651718812</v>
       </c>
       <c r="O24" s="8" t="s">
@@ -2668,13 +2633,13 @@
         <v>18</v>
       </c>
       <c r="R24" s="6">
-        <f t="shared" si="7"/>
+        <f>((L24/$L$32)*$P$2)/C24</f>
         <v>69.067093748212542</v>
       </c>
       <c r="S24" s="2"/>
       <c r="T24" s="7"/>
       <c r="U24" s="17">
-        <f t="shared" si="8"/>
+        <f t="shared" si="6"/>
         <v>1096.6195732997769</v>
       </c>
       <c r="V24" s="6"/>
@@ -2685,11 +2650,11 @@
         <v>1100</v>
       </c>
       <c r="AA24" s="10">
+        <f t="shared" si="2"/>
+        <v>2867.7000514785796</v>
+      </c>
+      <c r="AB24" s="11">
         <f t="shared" si="3"/>
-        <v>2867.7000514785796</v>
-      </c>
-      <c r="AB24" s="11">
-        <f t="shared" si="4"/>
         <v>1.4655235411557341</v>
       </c>
     </row>
@@ -2703,7 +2668,9 @@
       <c r="C25" s="3">
         <v>33</v>
       </c>
-      <c r="D25" s="31"/>
+      <c r="D25" s="31" t="s">
+        <v>78</v>
+      </c>
       <c r="E25" s="31"/>
       <c r="F25" s="31"/>
       <c r="G25" s="31"/>
@@ -2714,23 +2681,23 @@
         <v>2800</v>
       </c>
       <c r="J25" s="6">
+        <f t="shared" si="7"/>
+        <v>92400</v>
+      </c>
+      <c r="K25" s="6">
+        <f>(J25/$J$32)*$M$2</f>
+        <v>449.23640107533032</v>
+      </c>
+      <c r="L25" s="6">
+        <f t="shared" si="8"/>
+        <v>92849.236401075337</v>
+      </c>
+      <c r="M25" s="6">
         <f t="shared" si="9"/>
-        <v>92400</v>
-      </c>
-      <c r="K25" s="6">
-        <f t="shared" si="1"/>
-        <v>449.23640107533032</v>
-      </c>
-      <c r="L25" s="6">
+        <v>2813.61322427501</v>
+      </c>
+      <c r="N25" s="6">
         <f t="shared" si="10"/>
-        <v>92849.236401075337</v>
-      </c>
-      <c r="M25" s="6">
-        <f t="shared" si="11"/>
-        <v>2813.61322427501</v>
-      </c>
-      <c r="N25" s="6">
-        <f t="shared" si="12"/>
         <v>1406.806612137505</v>
       </c>
       <c r="O25" s="8" t="s">
@@ -2743,13 +2710,13 @@
         <v>18</v>
       </c>
       <c r="R25" s="6">
-        <f t="shared" si="7"/>
+        <f>((L25/$L$32)*$P$2)/C25</f>
         <v>552.53674998570034</v>
       </c>
       <c r="S25" s="2"/>
       <c r="T25" s="7"/>
       <c r="U25" s="17">
-        <f t="shared" si="8"/>
+        <f t="shared" si="6"/>
         <v>5272.9565863982152</v>
       </c>
       <c r="V25" s="6"/>
@@ -2760,11 +2727,11 @@
         <v>5400</v>
       </c>
       <c r="AA25" s="10">
+        <f t="shared" si="2"/>
+        <v>50617.050849396561</v>
+      </c>
+      <c r="AB25" s="11">
         <f t="shared" si="3"/>
-        <v>50617.050849396561</v>
-      </c>
-      <c r="AB25" s="11">
-        <f t="shared" si="4"/>
         <v>2.3491105537149215</v>
       </c>
     </row>
@@ -2778,7 +2745,9 @@
       <c r="C26" s="3">
         <v>2</v>
       </c>
-      <c r="D26" s="31"/>
+      <c r="D26" s="31" t="s">
+        <v>77</v>
+      </c>
       <c r="E26" s="31"/>
       <c r="F26" s="31"/>
       <c r="G26" s="31"/>
@@ -2789,23 +2758,23 @@
         <v>3500</v>
       </c>
       <c r="J26" s="6">
+        <f t="shared" si="7"/>
+        <v>7000</v>
+      </c>
+      <c r="K26" s="6">
+        <f>(J26/$J$32)*$M$2</f>
+        <v>34.033060687525023</v>
+      </c>
+      <c r="L26" s="6">
+        <f t="shared" si="8"/>
+        <v>7034.033060687525</v>
+      </c>
+      <c r="M26" s="6">
         <f t="shared" si="9"/>
-        <v>7000</v>
-      </c>
-      <c r="K26" s="6">
-        <f t="shared" si="1"/>
-        <v>34.033060687525023</v>
-      </c>
-      <c r="L26" s="6">
+        <v>3517.0165303437625</v>
+      </c>
+      <c r="N26" s="6">
         <f t="shared" si="10"/>
-        <v>7034.033060687525</v>
-      </c>
-      <c r="M26" s="6">
-        <f t="shared" si="11"/>
-        <v>3517.0165303437625</v>
-      </c>
-      <c r="N26" s="6">
-        <f t="shared" si="12"/>
         <v>1758.5082651718812</v>
       </c>
       <c r="O26" s="8" t="s">
@@ -2818,13 +2787,13 @@
         <v>18</v>
       </c>
       <c r="R26" s="6">
-        <f t="shared" si="7"/>
+        <f>((L26/$L$32)*$P$2)/C26</f>
         <v>690.6709374821254</v>
       </c>
       <c r="S26" s="2"/>
       <c r="T26" s="7"/>
       <c r="U26" s="17">
-        <f t="shared" si="8"/>
+        <f t="shared" si="6"/>
         <v>6466.1957329977695</v>
       </c>
       <c r="V26" s="6"/>
@@ -2835,11 +2804,11 @@
         <v>6500</v>
       </c>
       <c r="AA26" s="10">
+        <f t="shared" si="2"/>
+        <v>3584.6250643482244</v>
+      </c>
+      <c r="AB26" s="11">
         <f t="shared" si="3"/>
-        <v>3584.6250643482244</v>
-      </c>
-      <c r="AB26" s="11">
-        <f t="shared" si="4"/>
         <v>0.66402131818880172</v>
       </c>
     </row>
@@ -2853,7 +2822,9 @@
       <c r="C27" s="3">
         <v>2</v>
       </c>
-      <c r="D27" s="31"/>
+      <c r="D27" s="31" t="s">
+        <v>77</v>
+      </c>
       <c r="E27" s="31"/>
       <c r="F27" s="31"/>
       <c r="G27" s="31"/>
@@ -2864,23 +2835,23 @@
         <v>5000</v>
       </c>
       <c r="J27" s="6">
+        <f t="shared" si="7"/>
+        <v>10000</v>
+      </c>
+      <c r="K27" s="6">
+        <f>(J27/$J$32)*$M$2</f>
+        <v>48.618658125035751</v>
+      </c>
+      <c r="L27" s="6">
+        <f t="shared" si="8"/>
+        <v>10048.618658125035</v>
+      </c>
+      <c r="M27" s="6">
         <f t="shared" si="9"/>
-        <v>10000</v>
-      </c>
-      <c r="K27" s="6">
-        <f t="shared" si="1"/>
-        <v>48.618658125035751</v>
-      </c>
-      <c r="L27" s="6">
+        <v>5024.3093290625175</v>
+      </c>
+      <c r="N27" s="6">
         <f t="shared" si="10"/>
-        <v>10048.618658125035</v>
-      </c>
-      <c r="M27" s="6">
-        <f t="shared" si="11"/>
-        <v>5024.3093290625175</v>
-      </c>
-      <c r="N27" s="6">
-        <f t="shared" si="12"/>
         <v>2512.1546645312587</v>
       </c>
       <c r="O27" s="8" t="s">
@@ -2893,13 +2864,13 @@
         <v>18</v>
       </c>
       <c r="R27" s="6">
-        <f t="shared" si="7"/>
+        <f>((L27/$L$32)*$P$2)/C27</f>
         <v>986.67276783160753</v>
       </c>
       <c r="S27" s="2"/>
       <c r="T27" s="7"/>
       <c r="U27" s="17">
-        <f t="shared" si="8"/>
+        <f t="shared" si="6"/>
         <v>9023.1367614253832</v>
       </c>
       <c r="V27" s="6"/>
@@ -2910,11 +2881,11 @@
         <v>9200</v>
       </c>
       <c r="AA27" s="10">
+        <f t="shared" si="2"/>
+        <v>5378.0358062117502</v>
+      </c>
+      <c r="AB27" s="11">
         <f t="shared" si="3"/>
-        <v>5378.0358062117502</v>
-      </c>
-      <c r="AB27" s="11">
-        <f t="shared" si="4"/>
         <v>0.7172957282301472</v>
       </c>
     </row>
@@ -2928,7 +2899,9 @@
       <c r="C28" s="3">
         <v>12</v>
       </c>
-      <c r="D28" s="31"/>
+      <c r="D28" s="31" t="s">
+        <v>75</v>
+      </c>
       <c r="E28" s="31"/>
       <c r="F28" s="31"/>
       <c r="G28" s="31"/>
@@ -2939,23 +2912,23 @@
         <v>450</v>
       </c>
       <c r="J28" s="6">
-        <f t="shared" ref="J28:J29" si="13">+I28*C28</f>
+        <f t="shared" ref="J28:J29" si="11">+I28*C28</f>
         <v>5400</v>
       </c>
       <c r="K28" s="6">
-        <f t="shared" si="1"/>
+        <f>(J28/$J$32)*$M$2</f>
         <v>26.254075387519304</v>
       </c>
       <c r="L28" s="6">
-        <f t="shared" ref="L28:L29" si="14">(J28+K28)</f>
+        <f t="shared" ref="L28:L29" si="12">(J28+K28)</f>
         <v>5426.2540753875192</v>
       </c>
       <c r="M28" s="6">
-        <f t="shared" ref="M28:M29" si="15">+L28/C28</f>
+        <f t="shared" ref="M28:M29" si="13">+L28/C28</f>
         <v>452.18783961562661</v>
       </c>
       <c r="N28" s="6">
-        <f t="shared" ref="N28:N29" si="16">+M28*0.5</f>
+        <f t="shared" ref="N28:N29" si="14">+M28*0.5</f>
         <v>226.09391980781331</v>
       </c>
       <c r="O28" s="8" t="s">
@@ -2968,13 +2941,13 @@
         <v>18</v>
       </c>
       <c r="R28" s="6">
-        <f t="shared" si="7"/>
+        <f>((L28/$L$32)*$P$2)/C28</f>
         <v>88.800549104844677</v>
       </c>
       <c r="S28" s="2"/>
       <c r="T28" s="7"/>
       <c r="U28" s="17">
-        <f t="shared" si="8"/>
+        <f t="shared" si="6"/>
         <v>1267.0823085282848</v>
       </c>
       <c r="V28" s="6"/>
@@ -2985,11 +2958,11 @@
         <v>1300</v>
       </c>
       <c r="AA28" s="10">
+        <f t="shared" si="2"/>
+        <v>3108.139335354344</v>
+      </c>
+      <c r="AB28" s="11">
         <f t="shared" si="3"/>
-        <v>3108.139335354344</v>
-      </c>
-      <c r="AB28" s="11">
-        <f t="shared" si="4"/>
         <v>1.5403647125188862</v>
       </c>
     </row>
@@ -3003,7 +2976,9 @@
       <c r="C29" s="3">
         <v>20</v>
       </c>
-      <c r="D29" s="31"/>
+      <c r="D29" s="31" t="s">
+        <v>75</v>
+      </c>
       <c r="E29" s="31"/>
       <c r="F29" s="31"/>
       <c r="G29" s="31"/>
@@ -3014,23 +2989,23 @@
         <v>350</v>
       </c>
       <c r="J29" s="6">
+        <f t="shared" si="11"/>
+        <v>7000</v>
+      </c>
+      <c r="K29" s="6">
+        <f>(J29/$J$32)*$M$2</f>
+        <v>34.033060687525023</v>
+      </c>
+      <c r="L29" s="6">
+        <f t="shared" si="12"/>
+        <v>7034.033060687525</v>
+      </c>
+      <c r="M29" s="6">
         <f t="shared" si="13"/>
-        <v>7000</v>
-      </c>
-      <c r="K29" s="6">
-        <f t="shared" si="1"/>
-        <v>34.033060687525023</v>
-      </c>
-      <c r="L29" s="6">
+        <v>351.70165303437625</v>
+      </c>
+      <c r="N29" s="6">
         <f t="shared" si="14"/>
-        <v>7034.033060687525</v>
-      </c>
-      <c r="M29" s="6">
-        <f t="shared" si="15"/>
-        <v>351.70165303437625</v>
-      </c>
-      <c r="N29" s="6">
-        <f t="shared" si="16"/>
         <v>175.85082651718812</v>
       </c>
       <c r="O29" s="8" t="s">
@@ -3043,13 +3018,13 @@
         <v>18</v>
       </c>
       <c r="R29" s="6">
-        <f t="shared" si="7"/>
+        <f>((L29/$L$32)*$P$2)/C29</f>
         <v>69.067093748212542</v>
       </c>
       <c r="S29" s="2"/>
       <c r="T29" s="7"/>
       <c r="U29" s="17">
-        <f t="shared" si="8"/>
+        <f t="shared" si="6"/>
         <v>1096.6195732997769</v>
       </c>
       <c r="V29" s="6"/>
@@ -3060,11 +3035,11 @@
         <v>1100</v>
       </c>
       <c r="AA29" s="10">
+        <f t="shared" si="2"/>
+        <v>3584.6250643482244</v>
+      </c>
+      <c r="AB29" s="11">
         <f t="shared" si="3"/>
-        <v>3584.6250643482244</v>
-      </c>
-      <c r="AB29" s="11">
-        <f t="shared" si="4"/>
         <v>1.6052643038091414</v>
       </c>
     </row>
@@ -3078,7 +3053,9 @@
       <c r="C30" s="3">
         <v>34</v>
       </c>
-      <c r="D30" s="31"/>
+      <c r="D30" s="31" t="s">
+        <v>75</v>
+      </c>
       <c r="E30" s="31"/>
       <c r="F30" s="31"/>
       <c r="G30" s="31"/>
@@ -3089,23 +3066,23 @@
         <v>300</v>
       </c>
       <c r="J30" s="6">
+        <f t="shared" si="7"/>
+        <v>10200</v>
+      </c>
+      <c r="K30" s="6">
+        <f>(J30/$J$32)*$M$2</f>
+        <v>49.59103128753646</v>
+      </c>
+      <c r="L30" s="6">
+        <f t="shared" si="8"/>
+        <v>10249.591031287537</v>
+      </c>
+      <c r="M30" s="6">
         <f t="shared" si="9"/>
-        <v>10200</v>
-      </c>
-      <c r="K30" s="6">
-        <f t="shared" si="1"/>
-        <v>49.59103128753646</v>
-      </c>
-      <c r="L30" s="6">
+        <v>301.4585597437511</v>
+      </c>
+      <c r="N30" s="6">
         <f t="shared" si="10"/>
-        <v>10249.591031287537</v>
-      </c>
-      <c r="M30" s="6">
-        <f t="shared" si="11"/>
-        <v>301.4585597437511</v>
-      </c>
-      <c r="N30" s="6">
-        <f t="shared" si="12"/>
         <v>150.72927987187555</v>
       </c>
       <c r="O30" s="8" t="s">
@@ -3118,13 +3095,13 @@
         <v>18</v>
       </c>
       <c r="R30" s="6">
-        <f t="shared" si="7"/>
+        <f>((L30/$L$32)*$P$2)/C30</f>
         <v>59.200366069896461</v>
       </c>
       <c r="S30" s="2"/>
       <c r="T30" s="7"/>
       <c r="U30" s="17">
-        <f t="shared" si="8"/>
+        <f t="shared" si="6"/>
         <v>1011.3882056855231</v>
       </c>
       <c r="V30" s="6"/>
@@ -3135,11 +3112,11 @@
         <v>1100</v>
       </c>
       <c r="AA30" s="10">
+        <f t="shared" si="2"/>
+        <v>8137.5965223359835</v>
+      </c>
+      <c r="AB30" s="11">
         <f t="shared" si="3"/>
-        <v>8137.5965223359835</v>
-      </c>
-      <c r="AB30" s="11">
-        <f t="shared" si="4"/>
         <v>2.891546871157415</v>
       </c>
     </row>
@@ -3153,7 +3130,9 @@
       <c r="C31" s="4">
         <v>20</v>
       </c>
-      <c r="D31" s="31"/>
+      <c r="D31" s="31" t="s">
+        <v>75</v>
+      </c>
       <c r="E31" s="31"/>
       <c r="F31" s="31"/>
       <c r="G31" s="31"/>
@@ -3164,23 +3143,23 @@
         <v>700</v>
       </c>
       <c r="J31" s="6">
+        <f t="shared" si="7"/>
+        <v>14000</v>
+      </c>
+      <c r="K31" s="6">
+        <f>(J31/$J$32)*$M$2</f>
+        <v>68.066121375050045</v>
+      </c>
+      <c r="L31" s="6">
+        <f t="shared" si="8"/>
+        <v>14068.06612137505</v>
+      </c>
+      <c r="M31" s="6">
         <f t="shared" si="9"/>
-        <v>14000</v>
-      </c>
-      <c r="K31" s="6">
-        <f t="shared" si="1"/>
-        <v>68.066121375050045</v>
-      </c>
-      <c r="L31" s="6">
+        <v>703.4033060687525</v>
+      </c>
+      <c r="N31" s="6">
         <f t="shared" si="10"/>
-        <v>14068.06612137505</v>
-      </c>
-      <c r="M31" s="6">
-        <f t="shared" si="11"/>
-        <v>703.4033060687525</v>
-      </c>
-      <c r="N31" s="6">
-        <f t="shared" si="12"/>
         <v>351.70165303437625</v>
       </c>
       <c r="O31" s="8" t="s">
@@ -3193,13 +3172,13 @@
         <v>18</v>
       </c>
       <c r="R31" s="6">
-        <f t="shared" si="7"/>
+        <f>((L31/$L$32)*$P$2)/C31</f>
         <v>138.13418749642508</v>
       </c>
       <c r="S31" s="2"/>
       <c r="T31" s="7"/>
       <c r="U31" s="17">
-        <f t="shared" si="8"/>
+        <f t="shared" si="6"/>
         <v>1693.2391465995538</v>
       </c>
       <c r="V31" s="27"/>
@@ -3210,11 +3189,11 @@
         <v>1700</v>
       </c>
       <c r="AA31" s="10">
+        <f t="shared" si="2"/>
+        <v>7169.2501286964489</v>
+      </c>
+      <c r="AB31" s="11">
         <f t="shared" si="3"/>
-        <v>7169.2501286964489</v>
-      </c>
-      <c r="AB31" s="11">
-        <f t="shared" si="4"/>
         <v>1.8076381147144978</v>
       </c>
     </row>
@@ -3307,13 +3286,13 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AB39"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:AB37"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane xSplit="1" topLeftCell="C1" activePane="topRight" state="frozen"/>
       <selection activeCell="B1" sqref="B1"/>
-      <selection pane="topRight" activeCell="A8" sqref="A8"/>
+      <selection pane="topRight" activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3346,7 +3325,7 @@
     </row>
     <row r="2" spans="1:28" ht="21" x14ac:dyDescent="0.4">
       <c r="A2" s="21" t="s">
-        <v>79</v>
+        <v>72</v>
       </c>
       <c r="B2" s="22"/>
       <c r="C2" s="34"/>
@@ -3368,8 +3347,8 @@
         <v>32</v>
       </c>
       <c r="P2" s="24">
-        <f>300*230</f>
-        <v>69000</v>
+        <f>50*230</f>
+        <v>11500</v>
       </c>
     </row>
     <row r="3" spans="1:28" ht="15.6" x14ac:dyDescent="0.3">
@@ -3468,45 +3447,45 @@
     </row>
     <row r="5" spans="1:28" ht="51.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="5">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="B5" s="25" t="s">
-        <v>80</v>
+        <v>73</v>
       </c>
       <c r="C5" s="3">
-        <v>30</v>
+        <v>15</v>
       </c>
       <c r="D5" s="31" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="E5" s="31"/>
       <c r="F5" s="31"/>
       <c r="G5" s="31"/>
       <c r="H5" s="31" t="s">
-        <v>29</v>
-      </c>
-      <c r="I5" s="15">
-        <v>350</v>
+        <v>36</v>
+      </c>
+      <c r="I5" s="13">
+        <v>5800</v>
       </c>
       <c r="J5" s="6">
-        <f t="shared" ref="J5:J30" si="0">+I5*C5</f>
-        <v>10500</v>
+        <f t="shared" ref="J5:J28" si="0">+I5*C5</f>
+        <v>87000</v>
       </c>
       <c r="K5" s="6">
-        <f t="shared" ref="K5:K30" si="1">(J5/$J$31)*$M$2</f>
-        <v>149.3099121706399</v>
+        <f>(J5/$J$29)*$M$2</f>
+        <v>1313.9658848614072</v>
       </c>
       <c r="L5" s="6">
-        <f>(J5+K5)</f>
-        <v>10649.30991217064</v>
+        <f t="shared" ref="L5:L28" si="1">(J5+K5)</f>
+        <v>88313.965884861405</v>
       </c>
       <c r="M5" s="6">
-        <f t="shared" ref="M5:M30" si="2">+L5/C5</f>
-        <v>354.97699707235466</v>
+        <f t="shared" ref="M5:M28" si="2">+L5/C5</f>
+        <v>5887.597725657427</v>
       </c>
       <c r="N5" s="6">
-        <f>+M5*0.5</f>
-        <v>177.48849853617733</v>
+        <f t="shared" ref="N5:N28" si="3">+M5*0.5</f>
+        <v>2943.7988628287135</v>
       </c>
       <c r="O5" s="8" t="s">
         <v>18</v>
@@ -3518,74 +3497,72 @@
         <v>18</v>
       </c>
       <c r="R5" s="6">
-        <f t="shared" ref="R5:R30" si="3">((L5/$L$31)*$P$2)/C5</f>
-        <v>202.00752823086574</v>
+        <f>((L5/$L$29)*$P$2)/C5</f>
+        <v>592.57285003553659</v>
       </c>
       <c r="S5" s="2"/>
       <c r="T5" s="7"/>
       <c r="U5" s="17">
-        <f>M5+P5+R5+S5+N5</f>
-        <v>1234.4730238393977</v>
+        <f t="shared" ref="U5:U28" si="4">M5+P5+R5+S5+N5</f>
+        <v>9923.9694385216771</v>
       </c>
       <c r="V5" s="6"/>
-      <c r="W5" s="6">
-        <v>1400</v>
-      </c>
+      <c r="W5" s="6"/>
       <c r="X5" s="6"/>
       <c r="Y5" s="28"/>
       <c r="Z5" s="9">
-        <v>1400</v>
+        <v>900</v>
       </c>
       <c r="AA5" s="10">
-        <f t="shared" ref="AA5:AA30" si="4">(Z5-M5-R5-P5)*C5</f>
-        <v>10290.464240903388</v>
+        <f t="shared" ref="AA5:AA28" si="5">(Z5-M5-R5-P5)*C5</f>
+        <v>-91202.558635394453</v>
       </c>
       <c r="AB5" s="11">
-        <f t="shared" ref="AB5:AB30" si="5">IFERROR(AA5/(M5+P5+R5*C5),"")</f>
-        <v>1.4880928980752075</v>
+        <f t="shared" ref="AB5:AB28" si="6">IFERROR(AA5/(M5+P5+R5*C5),"")</f>
+        <v>-5.9702423046860451</v>
       </c>
     </row>
     <row r="6" spans="1:28" ht="51.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="5">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="B6" s="25" t="s">
-        <v>82</v>
+        <v>74</v>
       </c>
       <c r="C6" s="3">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="D6" s="31" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="E6" s="31"/>
-      <c r="F6" s="31"/>
+      <c r="F6" s="31" t="s">
+        <v>36</v>
+      </c>
       <c r="G6" s="31"/>
-      <c r="H6" s="31" t="s">
-        <v>36</v>
-      </c>
+      <c r="H6" s="31"/>
       <c r="I6" s="13">
-        <v>1350</v>
+        <v>1800</v>
       </c>
       <c r="J6" s="6">
-        <f t="shared" si="0"/>
-        <v>4050</v>
+        <f>+I6*C6</f>
+        <v>18000</v>
       </c>
       <c r="K6" s="6">
+        <f>(J6/$J$29)*$M$2</f>
+        <v>271.85501066098084</v>
+      </c>
+      <c r="L6" s="6">
         <f t="shared" si="1"/>
-        <v>57.590966122961106</v>
-      </c>
-      <c r="L6" s="6">
-        <f t="shared" ref="L6:L30" si="6">(J6+K6)</f>
-        <v>4107.5909661229607</v>
+        <v>18271.85501066098</v>
       </c>
       <c r="M6" s="6">
         <f t="shared" si="2"/>
-        <v>1369.1969887076536</v>
+        <v>1827.1855010660979</v>
       </c>
       <c r="N6" s="6">
-        <f t="shared" ref="N6:N30" si="7">+M6*0.5</f>
-        <v>684.59849435382682</v>
+        <f t="shared" si="3"/>
+        <v>913.59275053304896</v>
       </c>
       <c r="O6" s="8" t="s">
         <v>18</v>
@@ -3597,45 +3574,45 @@
         <v>18</v>
       </c>
       <c r="R6" s="6">
-        <f t="shared" si="3"/>
-        <v>779.17189460476777</v>
+        <f>((L6/$L$29)*$P$2)/C6</f>
+        <v>183.90191897654586</v>
       </c>
       <c r="S6" s="2"/>
       <c r="T6" s="7"/>
       <c r="U6" s="17">
-        <f t="shared" ref="U6:U30" si="8">M6+P6+R6+S6+N6</f>
-        <v>3332.9673776662485</v>
+        <f t="shared" si="4"/>
+        <v>3424.6801705756925</v>
       </c>
       <c r="V6" s="6"/>
-      <c r="W6" s="6"/>
+      <c r="W6" s="6">
+        <v>9500</v>
+      </c>
       <c r="X6" s="6"/>
-      <c r="Y6" s="28">
-        <v>25000</v>
-      </c>
+      <c r="Y6" s="28"/>
       <c r="Z6" s="9">
-        <v>1300</v>
+        <v>8500</v>
       </c>
       <c r="AA6" s="10">
-        <f t="shared" si="4"/>
-        <v>-4045.1066499372646</v>
+        <f t="shared" si="5"/>
+        <v>59889.125799573558</v>
       </c>
       <c r="AB6" s="11">
-        <f t="shared" si="5"/>
-        <v>-0.96158377451345922</v>
+        <f t="shared" si="6"/>
+        <v>14.374984006755545</v>
       </c>
     </row>
     <row r="7" spans="1:28" ht="51.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="5">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="B7" s="25" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="C7" s="3">
-        <v>15</v>
+        <v>6</v>
       </c>
       <c r="D7" s="31" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="E7" s="31"/>
       <c r="F7" s="31"/>
@@ -3644,27 +3621,27 @@
         <v>36</v>
       </c>
       <c r="I7" s="13">
-        <v>5800</v>
+        <v>1260</v>
       </c>
       <c r="J7" s="6">
         <f t="shared" si="0"/>
-        <v>87000</v>
+        <v>7560</v>
       </c>
       <c r="K7" s="6">
+        <f>(J7/$J$29)*$M$2</f>
+        <v>114.17910447761194</v>
+      </c>
+      <c r="L7" s="6">
         <f t="shared" si="1"/>
-        <v>1237.1392722710164</v>
-      </c>
-      <c r="L7" s="6">
-        <f t="shared" si="6"/>
-        <v>88237.139272271015</v>
+        <v>7674.1791044776119</v>
       </c>
       <c r="M7" s="6">
         <f t="shared" si="2"/>
-        <v>5882.4759514847347</v>
+        <v>1279.0298507462687</v>
       </c>
       <c r="N7" s="6">
-        <f t="shared" si="7"/>
-        <v>2941.2379757423673</v>
+        <f t="shared" si="3"/>
+        <v>639.51492537313436</v>
       </c>
       <c r="O7" s="8" t="s">
         <v>18</v>
@@ -3676,72 +3653,64 @@
         <v>18</v>
       </c>
       <c r="R7" s="6">
-        <f t="shared" si="3"/>
-        <v>3347.5533249686323</v>
+        <f>((L7/$L$29)*$P$2)/C7</f>
+        <v>128.73134328358211</v>
       </c>
       <c r="S7" s="2"/>
       <c r="T7" s="7"/>
       <c r="U7" s="17">
-        <f t="shared" si="8"/>
-        <v>12671.267252195734</v>
+        <f t="shared" si="4"/>
+        <v>2547.2761194029854</v>
       </c>
       <c r="V7" s="6"/>
       <c r="W7" s="6"/>
       <c r="X7" s="6"/>
       <c r="Y7" s="28"/>
       <c r="Z7" s="9">
-        <v>900</v>
+        <v>1400</v>
       </c>
       <c r="AA7" s="10">
-        <f t="shared" si="4"/>
-        <v>-132450.43914680049</v>
+        <f t="shared" si="5"/>
+        <v>-3046.567164179105</v>
       </c>
       <c r="AB7" s="11">
-        <f t="shared" si="5"/>
-        <v>-2.3402884263655546</v>
+        <f t="shared" si="6"/>
+        <v>-1.1940682675714411</v>
       </c>
     </row>
     <row r="8" spans="1:28" ht="51.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="5">
-        <v>5</v>
-      </c>
-      <c r="B8" s="25" t="s">
-        <v>84</v>
-      </c>
-      <c r="C8" s="3">
-        <v>10</v>
-      </c>
-      <c r="D8" s="31" t="s">
-        <v>85</v>
-      </c>
+        <v>7</v>
+      </c>
+      <c r="B8" s="25"/>
+      <c r="C8" s="3"/>
+      <c r="D8" s="31"/>
       <c r="E8" s="31"/>
-      <c r="F8" s="31" t="s">
+      <c r="F8" s="31"/>
+      <c r="G8" s="31"/>
+      <c r="H8" s="31" t="s">
         <v>36</v>
       </c>
-      <c r="G8" s="31"/>
-      <c r="H8" s="31"/>
-      <c r="I8" s="13">
-        <v>1800</v>
-      </c>
+      <c r="I8" s="13"/>
       <c r="J8" s="6">
-        <f>+I8*C8</f>
-        <v>18000</v>
+        <f t="shared" si="0"/>
+        <v>0</v>
       </c>
       <c r="K8" s="6">
+        <f>(J8/$J$29)*$M$2</f>
+        <v>0</v>
+      </c>
+      <c r="L8" s="6">
         <f t="shared" si="1"/>
-        <v>255.95984943538267</v>
-      </c>
-      <c r="L8" s="6">
-        <f t="shared" si="6"/>
-        <v>18255.959849435381</v>
-      </c>
-      <c r="M8" s="6">
+        <v>0</v>
+      </c>
+      <c r="M8" s="6" t="e">
         <f t="shared" si="2"/>
-        <v>1825.595984943538</v>
-      </c>
-      <c r="N8" s="6">
-        <f t="shared" si="7"/>
-        <v>912.79799247176902</v>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="N8" s="6" t="e">
+        <f t="shared" si="3"/>
+        <v>#DIV/0!</v>
       </c>
       <c r="O8" s="8" t="s">
         <v>18</v>
@@ -3752,37 +3721,35 @@
       <c r="Q8" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="R8" s="6">
-        <f t="shared" si="3"/>
-        <v>1038.8958594730238</v>
+      <c r="R8" s="6" t="e">
+        <f>((L8/$L$29)*$P$2)/C8</f>
+        <v>#DIV/0!</v>
       </c>
       <c r="S8" s="2"/>
       <c r="T8" s="7"/>
-      <c r="U8" s="17">
-        <f t="shared" si="8"/>
-        <v>4277.2898368883307</v>
+      <c r="U8" s="17" t="e">
+        <f t="shared" si="4"/>
+        <v>#DIV/0!</v>
       </c>
       <c r="V8" s="6"/>
-      <c r="W8" s="6">
-        <v>9500</v>
-      </c>
+      <c r="W8" s="6"/>
       <c r="X8" s="6"/>
       <c r="Y8" s="28"/>
       <c r="Z8" s="9">
-        <v>8500</v>
-      </c>
-      <c r="AA8" s="10">
-        <f t="shared" si="4"/>
-        <v>51355.081555834375</v>
-      </c>
-      <c r="AB8" s="11">
+        <v>1100</v>
+      </c>
+      <c r="AA8" s="10" t="e">
         <f t="shared" si="5"/>
-        <v>4.0390783046331471</v>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AB8" s="11" t="str">
+        <f t="shared" si="6"/>
+        <v/>
       </c>
     </row>
     <row r="9" spans="1:28" ht="51.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="5">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="B9" s="25"/>
       <c r="C9" s="3"/>
@@ -3799,11 +3766,11 @@
         <v>0</v>
       </c>
       <c r="K9" s="6">
+        <f>(J9/$J$29)*$M$2</f>
+        <v>0</v>
+      </c>
+      <c r="L9" s="6">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="L9" s="6">
-        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="M9" s="6" t="e">
@@ -3811,7 +3778,7 @@
         <v>#DIV/0!</v>
       </c>
       <c r="N9" s="6" t="e">
-        <f t="shared" si="7"/>
+        <f t="shared" si="3"/>
         <v>#DIV/0!</v>
       </c>
       <c r="O9" s="8" t="s">
@@ -3824,13 +3791,13 @@
         <v>18</v>
       </c>
       <c r="R9" s="6" t="e">
-        <f t="shared" si="3"/>
+        <f>((L9/$L$29)*$P$2)/C9</f>
         <v>#DIV/0!</v>
       </c>
       <c r="S9" s="2"/>
       <c r="T9" s="7"/>
       <c r="U9" s="17" t="e">
-        <f t="shared" si="8"/>
+        <f t="shared" si="4"/>
         <v>#DIV/0!</v>
       </c>
       <c r="V9" s="6"/>
@@ -3838,20 +3805,20 @@
       <c r="X9" s="6"/>
       <c r="Y9" s="28"/>
       <c r="Z9" s="9">
-        <v>1400</v>
+        <v>1200</v>
       </c>
       <c r="AA9" s="10" t="e">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>#DIV/0!</v>
       </c>
       <c r="AB9" s="11" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
     </row>
     <row r="10" spans="1:28" ht="51.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="5">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="B10" s="25"/>
       <c r="C10" s="3"/>
@@ -3859,20 +3826,18 @@
       <c r="E10" s="31"/>
       <c r="F10" s="31"/>
       <c r="G10" s="31"/>
-      <c r="H10" s="31" t="s">
-        <v>36</v>
-      </c>
+      <c r="H10" s="31"/>
       <c r="I10" s="13"/>
       <c r="J10" s="6">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="K10" s="6">
+        <f>(J10/$J$29)*$M$2</f>
+        <v>0</v>
+      </c>
+      <c r="L10" s="6">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="L10" s="6">
-        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="M10" s="6" t="e">
@@ -3880,7 +3845,7 @@
         <v>#DIV/0!</v>
       </c>
       <c r="N10" s="6" t="e">
-        <f t="shared" si="7"/>
+        <f t="shared" si="3"/>
         <v>#DIV/0!</v>
       </c>
       <c r="O10" s="8" t="s">
@@ -3893,13 +3858,13 @@
         <v>18</v>
       </c>
       <c r="R10" s="6" t="e">
-        <f t="shared" si="3"/>
+        <f>((L10/$L$29)*$P$2)/C10</f>
         <v>#DIV/0!</v>
       </c>
       <c r="S10" s="2"/>
       <c r="T10" s="7"/>
       <c r="U10" s="17" t="e">
-        <f t="shared" si="8"/>
+        <f t="shared" si="4"/>
         <v>#DIV/0!</v>
       </c>
       <c r="V10" s="6"/>
@@ -3907,20 +3872,20 @@
       <c r="X10" s="6"/>
       <c r="Y10" s="28"/>
       <c r="Z10" s="9">
-        <v>1100</v>
+        <v>1350</v>
       </c>
       <c r="AA10" s="10" t="e">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>#DIV/0!</v>
       </c>
       <c r="AB10" s="11" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
     </row>
     <row r="11" spans="1:28" ht="51.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="5">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="B11" s="25"/>
       <c r="C11" s="3"/>
@@ -3937,11 +3902,11 @@
         <v>0</v>
       </c>
       <c r="K11" s="6">
+        <f>(J11/$J$29)*$M$2</f>
+        <v>0</v>
+      </c>
+      <c r="L11" s="6">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="L11" s="6">
-        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="M11" s="6" t="e">
@@ -3949,7 +3914,7 @@
         <v>#DIV/0!</v>
       </c>
       <c r="N11" s="6" t="e">
-        <f t="shared" si="7"/>
+        <f t="shared" si="3"/>
         <v>#DIV/0!</v>
       </c>
       <c r="O11" s="8" t="s">
@@ -3962,13 +3927,13 @@
         <v>18</v>
       </c>
       <c r="R11" s="6" t="e">
-        <f t="shared" si="3"/>
+        <f>((L11/$L$29)*$P$2)/C11</f>
         <v>#DIV/0!</v>
       </c>
       <c r="S11" s="2"/>
       <c r="T11" s="7"/>
       <c r="U11" s="17" t="e">
-        <f t="shared" si="8"/>
+        <f t="shared" si="4"/>
         <v>#DIV/0!</v>
       </c>
       <c r="V11" s="6"/>
@@ -3976,20 +3941,20 @@
       <c r="X11" s="6"/>
       <c r="Y11" s="28"/>
       <c r="Z11" s="9">
-        <v>1200</v>
+        <v>1700</v>
       </c>
       <c r="AA11" s="10" t="e">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>#DIV/0!</v>
       </c>
       <c r="AB11" s="11" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
     </row>
     <row r="12" spans="1:28" ht="51.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="5">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="B12" s="25"/>
       <c r="C12" s="3"/>
@@ -3997,18 +3962,20 @@
       <c r="E12" s="31"/>
       <c r="F12" s="31"/>
       <c r="G12" s="31"/>
-      <c r="H12" s="31"/>
+      <c r="H12" s="31" t="s">
+        <v>36</v>
+      </c>
       <c r="I12" s="13"/>
       <c r="J12" s="6">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="K12" s="6">
+        <f>(J12/$J$29)*$M$2</f>
+        <v>0</v>
+      </c>
+      <c r="L12" s="6">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="L12" s="6">
-        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="M12" s="6" t="e">
@@ -4016,7 +3983,7 @@
         <v>#DIV/0!</v>
       </c>
       <c r="N12" s="6" t="e">
-        <f t="shared" si="7"/>
+        <f t="shared" si="3"/>
         <v>#DIV/0!</v>
       </c>
       <c r="O12" s="8" t="s">
@@ -4029,13 +3996,13 @@
         <v>18</v>
       </c>
       <c r="R12" s="6" t="e">
-        <f t="shared" si="3"/>
+        <f>((L12/$L$29)*$P$2)/C12</f>
         <v>#DIV/0!</v>
       </c>
       <c r="S12" s="2"/>
       <c r="T12" s="7"/>
       <c r="U12" s="17" t="e">
-        <f t="shared" si="8"/>
+        <f t="shared" si="4"/>
         <v>#DIV/0!</v>
       </c>
       <c r="V12" s="6"/>
@@ -4043,20 +4010,20 @@
       <c r="X12" s="6"/>
       <c r="Y12" s="28"/>
       <c r="Z12" s="9">
-        <v>1350</v>
+        <v>1900</v>
       </c>
       <c r="AA12" s="10" t="e">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>#DIV/0!</v>
       </c>
       <c r="AB12" s="11" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
     </row>
     <row r="13" spans="1:28" ht="51.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="5">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="B13" s="25"/>
       <c r="C13" s="3"/>
@@ -4073,11 +4040,11 @@
         <v>0</v>
       </c>
       <c r="K13" s="6">
+        <f>(J13/$J$29)*$M$2</f>
+        <v>0</v>
+      </c>
+      <c r="L13" s="6">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="L13" s="6">
-        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="M13" s="6" t="e">
@@ -4085,7 +4052,7 @@
         <v>#DIV/0!</v>
       </c>
       <c r="N13" s="6" t="e">
-        <f t="shared" si="7"/>
+        <f t="shared" si="3"/>
         <v>#DIV/0!</v>
       </c>
       <c r="O13" s="8" t="s">
@@ -4098,13 +4065,13 @@
         <v>18</v>
       </c>
       <c r="R13" s="6" t="e">
-        <f t="shared" si="3"/>
+        <f>((L13/$L$29)*$P$2)/C13</f>
         <v>#DIV/0!</v>
       </c>
       <c r="S13" s="2"/>
       <c r="T13" s="7"/>
       <c r="U13" s="17" t="e">
-        <f t="shared" si="8"/>
+        <f t="shared" si="4"/>
         <v>#DIV/0!</v>
       </c>
       <c r="V13" s="6"/>
@@ -4112,20 +4079,20 @@
       <c r="X13" s="6"/>
       <c r="Y13" s="28"/>
       <c r="Z13" s="9">
-        <v>1700</v>
+        <v>1800</v>
       </c>
       <c r="AA13" s="10" t="e">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>#DIV/0!</v>
       </c>
       <c r="AB13" s="11" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
     </row>
     <row r="14" spans="1:28" ht="51.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="5">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="B14" s="25"/>
       <c r="C14" s="3"/>
@@ -4142,11 +4109,11 @@
         <v>0</v>
       </c>
       <c r="K14" s="6">
+        <f>(J14/$J$29)*$M$2</f>
+        <v>0</v>
+      </c>
+      <c r="L14" s="6">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="L14" s="6">
-        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="M14" s="6" t="e">
@@ -4154,7 +4121,7 @@
         <v>#DIV/0!</v>
       </c>
       <c r="N14" s="6" t="e">
-        <f t="shared" si="7"/>
+        <f t="shared" si="3"/>
         <v>#DIV/0!</v>
       </c>
       <c r="O14" s="8" t="s">
@@ -4167,13 +4134,13 @@
         <v>18</v>
       </c>
       <c r="R14" s="6" t="e">
-        <f t="shared" si="3"/>
+        <f>((L14/$L$29)*$P$2)/C14</f>
         <v>#DIV/0!</v>
       </c>
       <c r="S14" s="2"/>
       <c r="T14" s="7"/>
       <c r="U14" s="17" t="e">
-        <f t="shared" si="8"/>
+        <f t="shared" si="4"/>
         <v>#DIV/0!</v>
       </c>
       <c r="V14" s="6"/>
@@ -4181,20 +4148,20 @@
       <c r="X14" s="6"/>
       <c r="Y14" s="28"/>
       <c r="Z14" s="9">
-        <v>1900</v>
+        <v>2600</v>
       </c>
       <c r="AA14" s="10" t="e">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>#DIV/0!</v>
       </c>
       <c r="AB14" s="11" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
     </row>
     <row r="15" spans="1:28" ht="51.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="5">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="B15" s="25"/>
       <c r="C15" s="3"/>
@@ -4211,11 +4178,11 @@
         <v>0</v>
       </c>
       <c r="K15" s="6">
+        <f>(J15/$J$29)*$M$2</f>
+        <v>0</v>
+      </c>
+      <c r="L15" s="6">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="L15" s="6">
-        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="M15" s="6" t="e">
@@ -4223,7 +4190,7 @@
         <v>#DIV/0!</v>
       </c>
       <c r="N15" s="6" t="e">
-        <f t="shared" si="7"/>
+        <f t="shared" si="3"/>
         <v>#DIV/0!</v>
       </c>
       <c r="O15" s="8" t="s">
@@ -4236,13 +4203,13 @@
         <v>18</v>
       </c>
       <c r="R15" s="6" t="e">
-        <f t="shared" si="3"/>
+        <f>((L15/$L$29)*$P$2)/C15</f>
         <v>#DIV/0!</v>
       </c>
       <c r="S15" s="2"/>
       <c r="T15" s="7"/>
       <c r="U15" s="17" t="e">
-        <f t="shared" si="8"/>
+        <f t="shared" si="4"/>
         <v>#DIV/0!</v>
       </c>
       <c r="V15" s="6"/>
@@ -4250,20 +4217,20 @@
       <c r="X15" s="6"/>
       <c r="Y15" s="28"/>
       <c r="Z15" s="9">
-        <v>1800</v>
+        <v>1100</v>
       </c>
       <c r="AA15" s="10" t="e">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>#DIV/0!</v>
       </c>
       <c r="AB15" s="11" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
     </row>
     <row r="16" spans="1:28" ht="51.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="5">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="B16" s="25"/>
       <c r="C16" s="3"/>
@@ -4280,11 +4247,11 @@
         <v>0</v>
       </c>
       <c r="K16" s="6">
+        <f>(J16/$J$29)*$M$2</f>
+        <v>0</v>
+      </c>
+      <c r="L16" s="6">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="L16" s="6">
-        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="M16" s="6" t="e">
@@ -4292,7 +4259,7 @@
         <v>#DIV/0!</v>
       </c>
       <c r="N16" s="6" t="e">
-        <f t="shared" si="7"/>
+        <f t="shared" si="3"/>
         <v>#DIV/0!</v>
       </c>
       <c r="O16" s="8" t="s">
@@ -4305,13 +4272,13 @@
         <v>18</v>
       </c>
       <c r="R16" s="6" t="e">
-        <f t="shared" si="3"/>
+        <f>((L16/$L$29)*$P$2)/C16</f>
         <v>#DIV/0!</v>
       </c>
       <c r="S16" s="2"/>
       <c r="T16" s="7"/>
       <c r="U16" s="17" t="e">
-        <f t="shared" si="8"/>
+        <f t="shared" si="4"/>
         <v>#DIV/0!</v>
       </c>
       <c r="V16" s="6"/>
@@ -4319,20 +4286,20 @@
       <c r="X16" s="6"/>
       <c r="Y16" s="28"/>
       <c r="Z16" s="9">
-        <v>2600</v>
+        <v>2300</v>
       </c>
       <c r="AA16" s="10" t="e">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>#DIV/0!</v>
       </c>
       <c r="AB16" s="11" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
     </row>
     <row r="17" spans="1:28" ht="51.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="5">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="B17" s="25"/>
       <c r="C17" s="3"/>
@@ -4349,11 +4316,11 @@
         <v>0</v>
       </c>
       <c r="K17" s="6">
+        <f>(J17/$J$29)*$M$2</f>
+        <v>0</v>
+      </c>
+      <c r="L17" s="6">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="L17" s="6">
-        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="M17" s="6" t="e">
@@ -4361,7 +4328,7 @@
         <v>#DIV/0!</v>
       </c>
       <c r="N17" s="6" t="e">
-        <f t="shared" si="7"/>
+        <f t="shared" si="3"/>
         <v>#DIV/0!</v>
       </c>
       <c r="O17" s="8" t="s">
@@ -4374,13 +4341,13 @@
         <v>18</v>
       </c>
       <c r="R17" s="6" t="e">
-        <f t="shared" si="3"/>
+        <f>((L17/$L$29)*$P$2)/C17</f>
         <v>#DIV/0!</v>
       </c>
       <c r="S17" s="2"/>
       <c r="T17" s="7"/>
       <c r="U17" s="17" t="e">
-        <f t="shared" si="8"/>
+        <f t="shared" si="4"/>
         <v>#DIV/0!</v>
       </c>
       <c r="V17" s="6"/>
@@ -4391,17 +4358,17 @@
         <v>1100</v>
       </c>
       <c r="AA17" s="10" t="e">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>#DIV/0!</v>
       </c>
       <c r="AB17" s="11" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
     </row>
     <row r="18" spans="1:28" ht="51.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="5">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="B18" s="25"/>
       <c r="C18" s="3"/>
@@ -4418,11 +4385,11 @@
         <v>0</v>
       </c>
       <c r="K18" s="6">
+        <f>(J18/$J$29)*$M$2</f>
+        <v>0</v>
+      </c>
+      <c r="L18" s="6">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="L18" s="6">
-        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="M18" s="6" t="e">
@@ -4430,7 +4397,7 @@
         <v>#DIV/0!</v>
       </c>
       <c r="N18" s="6" t="e">
-        <f t="shared" si="7"/>
+        <f t="shared" si="3"/>
         <v>#DIV/0!</v>
       </c>
       <c r="O18" s="8" t="s">
@@ -4443,13 +4410,13 @@
         <v>18</v>
       </c>
       <c r="R18" s="6" t="e">
-        <f t="shared" si="3"/>
+        <f>((L18/$L$29)*$P$2)/C18</f>
         <v>#DIV/0!</v>
       </c>
       <c r="S18" s="2"/>
       <c r="T18" s="7"/>
       <c r="U18" s="17" t="e">
-        <f t="shared" si="8"/>
+        <f t="shared" si="4"/>
         <v>#DIV/0!</v>
       </c>
       <c r="V18" s="6"/>
@@ -4457,20 +4424,20 @@
       <c r="X18" s="6"/>
       <c r="Y18" s="28"/>
       <c r="Z18" s="9">
-        <v>2300</v>
+        <v>700</v>
       </c>
       <c r="AA18" s="10" t="e">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>#DIV/0!</v>
       </c>
       <c r="AB18" s="11" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
     </row>
     <row r="19" spans="1:28" ht="51.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="5">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="B19" s="25"/>
       <c r="C19" s="3"/>
@@ -4487,11 +4454,11 @@
         <v>0</v>
       </c>
       <c r="K19" s="6">
+        <f>(J19/$J$29)*$M$2</f>
+        <v>0</v>
+      </c>
+      <c r="L19" s="6">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="L19" s="6">
-        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="M19" s="6" t="e">
@@ -4499,7 +4466,7 @@
         <v>#DIV/0!</v>
       </c>
       <c r="N19" s="6" t="e">
-        <f t="shared" si="7"/>
+        <f t="shared" si="3"/>
         <v>#DIV/0!</v>
       </c>
       <c r="O19" s="8" t="s">
@@ -4512,13 +4479,13 @@
         <v>18</v>
       </c>
       <c r="R19" s="6" t="e">
-        <f t="shared" si="3"/>
+        <f>((L19/$L$29)*$P$2)/C19</f>
         <v>#DIV/0!</v>
       </c>
       <c r="S19" s="2"/>
       <c r="T19" s="7"/>
       <c r="U19" s="17" t="e">
-        <f t="shared" si="8"/>
+        <f t="shared" si="4"/>
         <v>#DIV/0!</v>
       </c>
       <c r="V19" s="6"/>
@@ -4526,20 +4493,20 @@
       <c r="X19" s="6"/>
       <c r="Y19" s="28"/>
       <c r="Z19" s="9">
-        <v>1100</v>
+        <v>800</v>
       </c>
       <c r="AA19" s="10" t="e">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>#DIV/0!</v>
       </c>
       <c r="AB19" s="11" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
     </row>
     <row r="20" spans="1:28" ht="51.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" s="5">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="B20" s="25"/>
       <c r="C20" s="3"/>
@@ -4556,11 +4523,11 @@
         <v>0</v>
       </c>
       <c r="K20" s="6">
+        <f>(J20/$J$29)*$M$2</f>
+        <v>0</v>
+      </c>
+      <c r="L20" s="6">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="L20" s="6">
-        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="M20" s="6" t="e">
@@ -4568,7 +4535,7 @@
         <v>#DIV/0!</v>
       </c>
       <c r="N20" s="6" t="e">
-        <f t="shared" si="7"/>
+        <f t="shared" si="3"/>
         <v>#DIV/0!</v>
       </c>
       <c r="O20" s="8" t="s">
@@ -4581,13 +4548,13 @@
         <v>18</v>
       </c>
       <c r="R20" s="6" t="e">
-        <f t="shared" si="3"/>
+        <f>((L20/$L$29)*$P$2)/C20</f>
         <v>#DIV/0!</v>
       </c>
       <c r="S20" s="2"/>
       <c r="T20" s="7"/>
       <c r="U20" s="17" t="e">
-        <f t="shared" si="8"/>
+        <f t="shared" si="4"/>
         <v>#DIV/0!</v>
       </c>
       <c r="V20" s="6"/>
@@ -4595,20 +4562,20 @@
       <c r="X20" s="6"/>
       <c r="Y20" s="28"/>
       <c r="Z20" s="9">
-        <v>700</v>
+        <v>800</v>
       </c>
       <c r="AA20" s="10" t="e">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>#DIV/0!</v>
       </c>
       <c r="AB20" s="11" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
     </row>
     <row r="21" spans="1:28" ht="51.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" s="5">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="B21" s="25"/>
       <c r="C21" s="3"/>
@@ -4625,11 +4592,11 @@
         <v>0</v>
       </c>
       <c r="K21" s="6">
+        <f>(J21/$J$29)*$M$2</f>
+        <v>0</v>
+      </c>
+      <c r="L21" s="6">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="L21" s="6">
-        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="M21" s="6" t="e">
@@ -4637,7 +4604,7 @@
         <v>#DIV/0!</v>
       </c>
       <c r="N21" s="6" t="e">
-        <f t="shared" si="7"/>
+        <f t="shared" si="3"/>
         <v>#DIV/0!</v>
       </c>
       <c r="O21" s="8" t="s">
@@ -4650,13 +4617,13 @@
         <v>18</v>
       </c>
       <c r="R21" s="6" t="e">
-        <f t="shared" si="3"/>
+        <f>((L21/$L$29)*$P$2)/C21</f>
         <v>#DIV/0!</v>
       </c>
       <c r="S21" s="2"/>
       <c r="T21" s="7"/>
       <c r="U21" s="17" t="e">
-        <f t="shared" si="8"/>
+        <f t="shared" si="4"/>
         <v>#DIV/0!</v>
       </c>
       <c r="V21" s="6"/>
@@ -4664,20 +4631,20 @@
       <c r="X21" s="6"/>
       <c r="Y21" s="28"/>
       <c r="Z21" s="9">
-        <v>800</v>
+        <v>1100</v>
       </c>
       <c r="AA21" s="10" t="e">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>#DIV/0!</v>
       </c>
       <c r="AB21" s="11" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
     </row>
     <row r="22" spans="1:28" ht="51.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" s="5">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="B22" s="25"/>
       <c r="C22" s="3"/>
@@ -4694,11 +4661,11 @@
         <v>0</v>
       </c>
       <c r="K22" s="6">
+        <f>(J22/$J$29)*$M$2</f>
+        <v>0</v>
+      </c>
+      <c r="L22" s="6">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="L22" s="6">
-        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="M22" s="6" t="e">
@@ -4706,7 +4673,7 @@
         <v>#DIV/0!</v>
       </c>
       <c r="N22" s="6" t="e">
-        <f t="shared" si="7"/>
+        <f t="shared" si="3"/>
         <v>#DIV/0!</v>
       </c>
       <c r="O22" s="8" t="s">
@@ -4719,13 +4686,13 @@
         <v>18</v>
       </c>
       <c r="R22" s="6" t="e">
-        <f t="shared" si="3"/>
+        <f>((L22/$L$29)*$P$2)/C22</f>
         <v>#DIV/0!</v>
       </c>
       <c r="S22" s="2"/>
       <c r="T22" s="7"/>
       <c r="U22" s="17" t="e">
-        <f t="shared" si="8"/>
+        <f t="shared" si="4"/>
         <v>#DIV/0!</v>
       </c>
       <c r="V22" s="6"/>
@@ -4733,20 +4700,20 @@
       <c r="X22" s="6"/>
       <c r="Y22" s="28"/>
       <c r="Z22" s="9">
-        <v>800</v>
+        <v>5400</v>
       </c>
       <c r="AA22" s="10" t="e">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>#DIV/0!</v>
       </c>
       <c r="AB22" s="11" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
     </row>
     <row r="23" spans="1:28" ht="51.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A23" s="5">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="B23" s="25"/>
       <c r="C23" s="3"/>
@@ -4755,7 +4722,7 @@
       <c r="F23" s="31"/>
       <c r="G23" s="31"/>
       <c r="H23" s="31" t="s">
-        <v>36</v>
+        <v>29</v>
       </c>
       <c r="I23" s="13"/>
       <c r="J23" s="6">
@@ -4763,11 +4730,11 @@
         <v>0</v>
       </c>
       <c r="K23" s="6">
+        <f>(J23/$J$29)*$M$2</f>
+        <v>0</v>
+      </c>
+      <c r="L23" s="6">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="L23" s="6">
-        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="M23" s="6" t="e">
@@ -4775,7 +4742,7 @@
         <v>#DIV/0!</v>
       </c>
       <c r="N23" s="6" t="e">
-        <f t="shared" si="7"/>
+        <f t="shared" si="3"/>
         <v>#DIV/0!</v>
       </c>
       <c r="O23" s="8" t="s">
@@ -4788,13 +4755,13 @@
         <v>18</v>
       </c>
       <c r="R23" s="6" t="e">
-        <f t="shared" si="3"/>
+        <f>((L23/$L$29)*$P$2)/C23</f>
         <v>#DIV/0!</v>
       </c>
       <c r="S23" s="2"/>
       <c r="T23" s="7"/>
       <c r="U23" s="17" t="e">
-        <f t="shared" si="8"/>
+        <f t="shared" si="4"/>
         <v>#DIV/0!</v>
       </c>
       <c r="V23" s="6"/>
@@ -4802,20 +4769,20 @@
       <c r="X23" s="6"/>
       <c r="Y23" s="28"/>
       <c r="Z23" s="9">
-        <v>1100</v>
+        <v>6500</v>
       </c>
       <c r="AA23" s="10" t="e">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>#DIV/0!</v>
       </c>
       <c r="AB23" s="11" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
     </row>
     <row r="24" spans="1:28" ht="51.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A24" s="5">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="B24" s="25"/>
       <c r="C24" s="3"/>
@@ -4824,7 +4791,7 @@
       <c r="F24" s="31"/>
       <c r="G24" s="31"/>
       <c r="H24" s="31" t="s">
-        <v>36</v>
+        <v>29</v>
       </c>
       <c r="I24" s="13"/>
       <c r="J24" s="6">
@@ -4832,11 +4799,11 @@
         <v>0</v>
       </c>
       <c r="K24" s="6">
+        <f>(J24/$J$29)*$M$2</f>
+        <v>0</v>
+      </c>
+      <c r="L24" s="6">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="L24" s="6">
-        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="M24" s="6" t="e">
@@ -4844,7 +4811,7 @@
         <v>#DIV/0!</v>
       </c>
       <c r="N24" s="6" t="e">
-        <f t="shared" si="7"/>
+        <f t="shared" si="3"/>
         <v>#DIV/0!</v>
       </c>
       <c r="O24" s="8" t="s">
@@ -4857,13 +4824,13 @@
         <v>18</v>
       </c>
       <c r="R24" s="6" t="e">
-        <f t="shared" si="3"/>
+        <f>((L24/$L$29)*$P$2)/C24</f>
         <v>#DIV/0!</v>
       </c>
       <c r="S24" s="2"/>
       <c r="T24" s="7"/>
       <c r="U24" s="17" t="e">
-        <f t="shared" si="8"/>
+        <f t="shared" si="4"/>
         <v>#DIV/0!</v>
       </c>
       <c r="V24" s="6"/>
@@ -4871,20 +4838,20 @@
       <c r="X24" s="6"/>
       <c r="Y24" s="28"/>
       <c r="Z24" s="9">
-        <v>5400</v>
+        <v>9200</v>
       </c>
       <c r="AA24" s="10" t="e">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>#DIV/0!</v>
       </c>
       <c r="AB24" s="11" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
     </row>
     <row r="25" spans="1:28" ht="51.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A25" s="5">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="B25" s="25"/>
       <c r="C25" s="3"/>
@@ -4893,7 +4860,7 @@
       <c r="F25" s="31"/>
       <c r="G25" s="31"/>
       <c r="H25" s="31" t="s">
-        <v>29</v>
+        <v>36</v>
       </c>
       <c r="I25" s="13"/>
       <c r="J25" s="6">
@@ -4901,11 +4868,11 @@
         <v>0</v>
       </c>
       <c r="K25" s="6">
+        <f>(J25/$J$29)*$M$2</f>
+        <v>0</v>
+      </c>
+      <c r="L25" s="6">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="L25" s="6">
-        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="M25" s="6" t="e">
@@ -4913,7 +4880,7 @@
         <v>#DIV/0!</v>
       </c>
       <c r="N25" s="6" t="e">
-        <f t="shared" si="7"/>
+        <f t="shared" si="3"/>
         <v>#DIV/0!</v>
       </c>
       <c r="O25" s="8" t="s">
@@ -4926,13 +4893,13 @@
         <v>18</v>
       </c>
       <c r="R25" s="6" t="e">
-        <f t="shared" si="3"/>
+        <f>((L25/$L$29)*$P$2)/C25</f>
         <v>#DIV/0!</v>
       </c>
       <c r="S25" s="2"/>
       <c r="T25" s="7"/>
       <c r="U25" s="17" t="e">
-        <f t="shared" si="8"/>
+        <f t="shared" si="4"/>
         <v>#DIV/0!</v>
       </c>
       <c r="V25" s="6"/>
@@ -4940,20 +4907,20 @@
       <c r="X25" s="6"/>
       <c r="Y25" s="28"/>
       <c r="Z25" s="9">
-        <v>6500</v>
+        <v>1300</v>
       </c>
       <c r="AA25" s="10" t="e">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>#DIV/0!</v>
       </c>
       <c r="AB25" s="11" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
     </row>
     <row r="26" spans="1:28" ht="51.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A26" s="5">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="B26" s="25"/>
       <c r="C26" s="3"/>
@@ -4962,7 +4929,7 @@
       <c r="F26" s="31"/>
       <c r="G26" s="31"/>
       <c r="H26" s="31" t="s">
-        <v>29</v>
+        <v>36</v>
       </c>
       <c r="I26" s="13"/>
       <c r="J26" s="6">
@@ -4970,11 +4937,11 @@
         <v>0</v>
       </c>
       <c r="K26" s="6">
+        <f>(J26/$J$29)*$M$2</f>
+        <v>0</v>
+      </c>
+      <c r="L26" s="6">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="L26" s="6">
-        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="M26" s="6" t="e">
@@ -4982,7 +4949,7 @@
         <v>#DIV/0!</v>
       </c>
       <c r="N26" s="6" t="e">
-        <f t="shared" si="7"/>
+        <f t="shared" si="3"/>
         <v>#DIV/0!</v>
       </c>
       <c r="O26" s="8" t="s">
@@ -4995,13 +4962,13 @@
         <v>18</v>
       </c>
       <c r="R26" s="6" t="e">
-        <f t="shared" si="3"/>
+        <f>((L26/$L$29)*$P$2)/C26</f>
         <v>#DIV/0!</v>
       </c>
       <c r="S26" s="2"/>
       <c r="T26" s="7"/>
       <c r="U26" s="17" t="e">
-        <f t="shared" si="8"/>
+        <f t="shared" si="4"/>
         <v>#DIV/0!</v>
       </c>
       <c r="V26" s="6"/>
@@ -5009,20 +4976,20 @@
       <c r="X26" s="6"/>
       <c r="Y26" s="28"/>
       <c r="Z26" s="9">
-        <v>9200</v>
+        <v>1100</v>
       </c>
       <c r="AA26" s="10" t="e">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>#DIV/0!</v>
       </c>
       <c r="AB26" s="11" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
     </row>
     <row r="27" spans="1:28" ht="51.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A27" s="5">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="B27" s="25"/>
       <c r="C27" s="3"/>
@@ -5031,7 +4998,7 @@
       <c r="F27" s="31"/>
       <c r="G27" s="31"/>
       <c r="H27" s="31" t="s">
-        <v>36</v>
+        <v>29</v>
       </c>
       <c r="I27" s="13"/>
       <c r="J27" s="6">
@@ -5039,11 +5006,11 @@
         <v>0</v>
       </c>
       <c r="K27" s="6">
+        <f>(J27/$J$29)*$M$2</f>
+        <v>0</v>
+      </c>
+      <c r="L27" s="6">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="L27" s="6">
-        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="M27" s="6" t="e">
@@ -5051,7 +5018,7 @@
         <v>#DIV/0!</v>
       </c>
       <c r="N27" s="6" t="e">
-        <f t="shared" si="7"/>
+        <f t="shared" si="3"/>
         <v>#DIV/0!</v>
       </c>
       <c r="O27" s="8" t="s">
@@ -5064,13 +5031,13 @@
         <v>18</v>
       </c>
       <c r="R27" s="6" t="e">
-        <f t="shared" si="3"/>
+        <f>((L27/$L$29)*$P$2)/C27</f>
         <v>#DIV/0!</v>
       </c>
       <c r="S27" s="2"/>
       <c r="T27" s="7"/>
       <c r="U27" s="17" t="e">
-        <f t="shared" si="8"/>
+        <f t="shared" si="4"/>
         <v>#DIV/0!</v>
       </c>
       <c r="V27" s="6"/>
@@ -5078,41 +5045,41 @@
       <c r="X27" s="6"/>
       <c r="Y27" s="28"/>
       <c r="Z27" s="9">
-        <v>1300</v>
+        <v>1100</v>
       </c>
       <c r="AA27" s="10" t="e">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>#DIV/0!</v>
       </c>
       <c r="AB27" s="11" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
     </row>
     <row r="28" spans="1:28" ht="51.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A28" s="5">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="B28" s="25"/>
-      <c r="C28" s="3"/>
+      <c r="C28" s="4"/>
       <c r="D28" s="31"/>
       <c r="E28" s="31"/>
       <c r="F28" s="31"/>
       <c r="G28" s="31"/>
       <c r="H28" s="31" t="s">
-        <v>36</v>
-      </c>
-      <c r="I28" s="13"/>
+        <v>29</v>
+      </c>
+      <c r="I28" s="14"/>
       <c r="J28" s="6">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="K28" s="6">
+        <f>(J28/$J$29)*$M$2</f>
+        <v>0</v>
+      </c>
+      <c r="L28" s="6">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="L28" s="6">
-        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="M28" s="6" t="e">
@@ -5120,7 +5087,7 @@
         <v>#DIV/0!</v>
       </c>
       <c r="N28" s="6" t="e">
-        <f t="shared" si="7"/>
+        <f t="shared" si="3"/>
         <v>#DIV/0!</v>
       </c>
       <c r="O28" s="8" t="s">
@@ -5133,232 +5100,94 @@
         <v>18</v>
       </c>
       <c r="R28" s="6" t="e">
-        <f t="shared" si="3"/>
+        <f>((L28/$L$29)*$P$2)/C28</f>
         <v>#DIV/0!</v>
       </c>
       <c r="S28" s="2"/>
       <c r="T28" s="7"/>
       <c r="U28" s="17" t="e">
-        <f t="shared" si="8"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="V28" s="6"/>
-      <c r="W28" s="6"/>
-      <c r="X28" s="6"/>
-      <c r="Y28" s="28"/>
+        <f t="shared" si="4"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="V28" s="27"/>
+      <c r="W28" s="27"/>
+      <c r="X28" s="27"/>
+      <c r="Y28" s="27"/>
       <c r="Z28" s="9">
-        <v>1100</v>
+        <v>1700</v>
       </c>
       <c r="AA28" s="10" t="e">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>#DIV/0!</v>
       </c>
       <c r="AB28" s="11" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
     </row>
-    <row r="29" spans="1:28" ht="51.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="5">
-        <v>26</v>
-      </c>
-      <c r="B29" s="25"/>
-      <c r="C29" s="3"/>
-      <c r="D29" s="31"/>
-      <c r="E29" s="31"/>
-      <c r="F29" s="31"/>
-      <c r="G29" s="31"/>
-      <c r="H29" s="31" t="s">
-        <v>29</v>
-      </c>
-      <c r="I29" s="13"/>
-      <c r="J29" s="6">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="K29" s="6">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="L29" s="6">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="M29" s="6" t="e">
-        <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="N29" s="6" t="e">
-        <f t="shared" si="7"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="O29" s="8" t="s">
-        <v>18</v>
-      </c>
-      <c r="P29" s="26">
-        <v>500</v>
-      </c>
-      <c r="Q29" s="8" t="s">
-        <v>18</v>
-      </c>
-      <c r="R29" s="6" t="e">
-        <f t="shared" si="3"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="S29" s="2"/>
-      <c r="T29" s="7"/>
-      <c r="U29" s="17" t="e">
-        <f t="shared" si="8"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="V29" s="6"/>
-      <c r="W29" s="6"/>
-      <c r="X29" s="6"/>
-      <c r="Y29" s="28"/>
-      <c r="Z29" s="9">
-        <v>1100</v>
-      </c>
-      <c r="AA29" s="10" t="e">
-        <f t="shared" si="4"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="AB29" s="11" t="str">
-        <f t="shared" si="5"/>
-        <v/>
-      </c>
-    </row>
-    <row r="30" spans="1:28" ht="51.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="5">
-        <v>27</v>
-      </c>
-      <c r="B30" s="25"/>
-      <c r="C30" s="4"/>
-      <c r="D30" s="31"/>
-      <c r="E30" s="31"/>
-      <c r="F30" s="31"/>
-      <c r="G30" s="31"/>
-      <c r="H30" s="31" t="s">
-        <v>29</v>
-      </c>
-      <c r="I30" s="14"/>
-      <c r="J30" s="6">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="K30" s="6">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="L30" s="6">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="M30" s="6" t="e">
-        <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="N30" s="6" t="e">
-        <f t="shared" si="7"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="O30" s="8" t="s">
-        <v>18</v>
-      </c>
-      <c r="P30" s="26">
-        <v>500</v>
-      </c>
-      <c r="Q30" s="8" t="s">
-        <v>18</v>
-      </c>
-      <c r="R30" s="6" t="e">
-        <f t="shared" si="3"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="S30" s="2"/>
-      <c r="T30" s="7"/>
-      <c r="U30" s="17" t="e">
-        <f t="shared" si="8"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="V30" s="27"/>
-      <c r="W30" s="27"/>
-      <c r="X30" s="27"/>
-      <c r="Y30" s="27"/>
-      <c r="Z30" s="9">
+    <row r="29" spans="1:28" ht="21.6" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="J29" s="35">
+        <f>SUM(J5:J28)</f>
+        <v>112560</v>
+      </c>
+      <c r="K29" s="35">
+        <f>SUM(K5:K28)</f>
         <v>1700</v>
       </c>
-      <c r="AA30" s="10" t="e">
-        <f t="shared" si="4"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="AB30" s="11" t="str">
-        <f t="shared" si="5"/>
-        <v/>
-      </c>
-    </row>
-    <row r="31" spans="1:28" ht="21.6" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="J31" s="35">
-        <f>SUM(J5:J30)</f>
-        <v>119550</v>
-      </c>
-      <c r="K31" s="35">
-        <f>SUM(K5:K30)</f>
-        <v>1700</v>
-      </c>
-      <c r="L31" s="35">
-        <f>SUM(L5:L30)</f>
-        <v>121250</v>
-      </c>
-      <c r="AA31" s="29" t="e">
-        <f>SUM(AA5:AA30)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="AB31" s="30">
-        <f>AVERAGE(AB5:AB30)</f>
-        <v>0.5563247504573352</v>
-      </c>
-    </row>
-    <row r="32" spans="1:28" ht="15" thickTop="1" x14ac:dyDescent="0.3"/>
-    <row r="33" spans="2:18" ht="15" x14ac:dyDescent="0.3">
-      <c r="B33" s="1" t="s">
+      <c r="L29" s="35">
+        <f>SUM(L5:L28)</f>
+        <v>114260</v>
+      </c>
+      <c r="AA29" s="29" t="e">
+        <f>SUM(AA5:AA28)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AB29" s="30">
+        <f>AVERAGE(AB5:AB28)</f>
+        <v>2.4035578114993532</v>
+      </c>
+    </row>
+    <row r="30" spans="1:28" ht="15" thickTop="1" x14ac:dyDescent="0.3"/>
+    <row r="31" spans="1:28" ht="15" x14ac:dyDescent="0.3">
+      <c r="B31" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C33" s="32"/>
-      <c r="D33" s="1"/>
-      <c r="E33" s="1"/>
-      <c r="F33" s="1"/>
-      <c r="G33" s="1"/>
-      <c r="H33" s="1"/>
-      <c r="I33" s="1"/>
-      <c r="L33" s="12"/>
-      <c r="M33" s="1"/>
-    </row>
-    <row r="36" spans="2:18" x14ac:dyDescent="0.3">
-      <c r="O36" t="s">
+      <c r="C31" s="32"/>
+      <c r="D31" s="1"/>
+      <c r="E31" s="1"/>
+      <c r="F31" s="1"/>
+      <c r="G31" s="1"/>
+      <c r="H31" s="1"/>
+      <c r="I31" s="1"/>
+      <c r="L31" s="12"/>
+      <c r="M31" s="1"/>
+    </row>
+    <row r="34" spans="15:18" x14ac:dyDescent="0.3">
+      <c r="O34" t="s">
         <v>61</v>
       </c>
-      <c r="P36" t="s">
+      <c r="P34" t="s">
         <v>65</v>
       </c>
-      <c r="Q36" t="s">
+      <c r="Q34" t="s">
         <v>66</v>
       </c>
-      <c r="R36" t="s">
+      <c r="R34" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="37" spans="2:18" x14ac:dyDescent="0.3">
+    <row r="35" spans="15:18" x14ac:dyDescent="0.3">
+      <c r="O35" s="36" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="36" spans="15:18" x14ac:dyDescent="0.3">
+      <c r="O36" s="36" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="37" spans="15:18" x14ac:dyDescent="0.3">
       <c r="O37" s="36" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="38" spans="2:18" x14ac:dyDescent="0.3">
-      <c r="O38" s="36" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="39" spans="2:18" x14ac:dyDescent="0.3">
-      <c r="O39" s="36" t="s">
         <v>64</v>
       </c>
     </row>
@@ -5368,6 +5197,5 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
-  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>